<commit_message>
https://jira.jda.com/browse/LRR-3399 baseline improvement in 24 cases, due to changes done by Ravi. 50220,50221,50222,50223,50224,50225,50226,50227,50229,50230,50231,50232,50233,50234,50235,50236,50240,50241,50242,50243,50245,50246,VOL-50514,VOL-50517
</commit_message>
<xml_diff>
--- a/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
+++ b/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\baseline\outputbaselines\1.TestCaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A3450D-FEEB-4CC6-B8B8-8CBF225C389A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F136E638-B1E2-42D6-9E68-FF30CDD2E967}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="538">
   <si>
     <t>S.No.</t>
   </si>
@@ -1668,13 +1668,16 @@
   </si>
   <si>
     <t>change in derived rank logic, current result in-line with expectation</t>
+  </si>
+  <si>
+    <t>Results better than before due to improvement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1693,6 +1696,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1715,7 +1724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1858,11 +1867,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1928,6 +1952,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2249,7 +2276,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2312,9 @@
       <c r="H1" s="16">
         <v>44456</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="16">
+        <v>44467</v>
+      </c>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
@@ -14375,7 +14404,7 @@
       <c r="T417" s="3"/>
       <c r="U417" s="5"/>
     </row>
-    <row r="418" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A418" s="12">
         <v>416</v>
       </c>
@@ -14406,7 +14435,7 @@
       <c r="T418" s="3"/>
       <c r="U418" s="5"/>
     </row>
-    <row r="419" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A419" s="12">
         <v>417</v>
       </c>
@@ -14423,7 +14452,9 @@
         <v>526</v>
       </c>
       <c r="H419" s="3"/>
-      <c r="I419" s="3"/>
+      <c r="I419" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J419" s="3"/>
       <c r="K419" s="3"/>
       <c r="L419" s="3"/>
@@ -14437,7 +14468,7 @@
       <c r="T419" s="3"/>
       <c r="U419" s="5"/>
     </row>
-    <row r="420" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A420" s="12">
         <v>418</v>
       </c>
@@ -14454,7 +14485,9 @@
         <v>526</v>
       </c>
       <c r="H420" s="3"/>
-      <c r="I420" s="3"/>
+      <c r="I420" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J420" s="3"/>
       <c r="K420" s="3"/>
       <c r="L420" s="3"/>
@@ -14468,7 +14501,7 @@
       <c r="T420" s="3"/>
       <c r="U420" s="5"/>
     </row>
-    <row r="421" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A421" s="12">
         <v>419</v>
       </c>
@@ -14485,7 +14518,9 @@
         <v>526</v>
       </c>
       <c r="H421" s="3"/>
-      <c r="I421" s="3"/>
+      <c r="I421" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J421" s="3"/>
       <c r="K421" s="3"/>
       <c r="L421" s="3"/>
@@ -14499,7 +14534,7 @@
       <c r="T421" s="3"/>
       <c r="U421" s="5"/>
     </row>
-    <row r="422" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A422" s="12">
         <v>420</v>
       </c>
@@ -14516,7 +14551,9 @@
         <v>526</v>
       </c>
       <c r="H422" s="3"/>
-      <c r="I422" s="3"/>
+      <c r="I422" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J422" s="3"/>
       <c r="K422" s="3"/>
       <c r="L422" s="3"/>
@@ -14530,7 +14567,7 @@
       <c r="T422" s="3"/>
       <c r="U422" s="5"/>
     </row>
-    <row r="423" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A423" s="12">
         <v>421</v>
       </c>
@@ -14547,7 +14584,9 @@
         <v>527</v>
       </c>
       <c r="H423" s="3"/>
-      <c r="I423" s="3"/>
+      <c r="I423" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J423" s="3"/>
       <c r="K423" s="3"/>
       <c r="L423" s="3"/>
@@ -14561,7 +14600,7 @@
       <c r="T423" s="3"/>
       <c r="U423" s="5"/>
     </row>
-    <row r="424" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A424" s="12">
         <v>422</v>
       </c>
@@ -14578,7 +14617,9 @@
         <v>515</v>
       </c>
       <c r="H424" s="3"/>
-      <c r="I424" s="3"/>
+      <c r="I424" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J424" s="3"/>
       <c r="K424" s="3"/>
       <c r="L424" s="3"/>
@@ -14592,7 +14633,7 @@
       <c r="T424" s="3"/>
       <c r="U424" s="5"/>
     </row>
-    <row r="425" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A425" s="12">
         <v>423</v>
       </c>
@@ -14609,7 +14650,9 @@
         <v>528</v>
       </c>
       <c r="H425" s="3"/>
-      <c r="I425" s="3"/>
+      <c r="I425" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J425" s="3"/>
       <c r="K425" s="3"/>
       <c r="L425" s="3"/>
@@ -14623,7 +14666,7 @@
       <c r="T425" s="3"/>
       <c r="U425" s="5"/>
     </row>
-    <row r="426" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A426" s="12">
         <v>424</v>
       </c>
@@ -14640,7 +14683,9 @@
         <v>529</v>
       </c>
       <c r="H426" s="3"/>
-      <c r="I426" s="3"/>
+      <c r="I426" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J426" s="3"/>
       <c r="K426" s="3"/>
       <c r="L426" s="3"/>
@@ -14654,7 +14699,7 @@
       <c r="T426" s="3"/>
       <c r="U426" s="5"/>
     </row>
-    <row r="427" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A427" s="12">
         <v>425</v>
       </c>
@@ -14671,7 +14716,9 @@
       </c>
       <c r="G427" s="3"/>
       <c r="H427" s="3"/>
-      <c r="I427" s="3"/>
+      <c r="I427" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J427" s="3"/>
       <c r="K427" s="3"/>
       <c r="L427" s="3"/>
@@ -14685,7 +14732,7 @@
       <c r="T427" s="3"/>
       <c r="U427" s="5"/>
     </row>
-    <row r="428" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A428" s="12">
         <v>426</v>
       </c>
@@ -14702,7 +14749,9 @@
         <v>515</v>
       </c>
       <c r="H428" s="3"/>
-      <c r="I428" s="3"/>
+      <c r="I428" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J428" s="3"/>
       <c r="K428" s="3"/>
       <c r="L428" s="3"/>
@@ -14716,7 +14765,7 @@
       <c r="T428" s="3"/>
       <c r="U428" s="5"/>
     </row>
-    <row r="429" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="12">
         <v>427</v>
       </c>
@@ -14735,7 +14784,9 @@
         <v>519</v>
       </c>
       <c r="H429" s="3"/>
-      <c r="I429" s="3"/>
+      <c r="I429" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J429" s="3"/>
       <c r="K429" s="3"/>
       <c r="L429" s="3"/>
@@ -14749,7 +14800,7 @@
       <c r="T429" s="3"/>
       <c r="U429" s="5"/>
     </row>
-    <row r="430" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A430" s="12">
         <v>428</v>
       </c>
@@ -14768,7 +14819,9 @@
         <v>519</v>
       </c>
       <c r="H430" s="3"/>
-      <c r="I430" s="3"/>
+      <c r="I430" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J430" s="3"/>
       <c r="K430" s="3"/>
       <c r="L430" s="3"/>
@@ -14782,7 +14835,7 @@
       <c r="T430" s="3"/>
       <c r="U430" s="5"/>
     </row>
-    <row r="431" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A431" s="12">
         <v>429</v>
       </c>
@@ -14799,7 +14852,9 @@
         <v>530</v>
       </c>
       <c r="H431" s="3"/>
-      <c r="I431" s="3"/>
+      <c r="I431" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J431" s="3"/>
       <c r="K431" s="3"/>
       <c r="L431" s="3"/>
@@ -14813,7 +14868,7 @@
       <c r="T431" s="3"/>
       <c r="U431" s="5"/>
     </row>
-    <row r="432" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A432" s="12">
         <v>430</v>
       </c>
@@ -14832,7 +14887,9 @@
         <v>519</v>
       </c>
       <c r="H432" s="3"/>
-      <c r="I432" s="3"/>
+      <c r="I432" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J432" s="3"/>
       <c r="K432" s="3"/>
       <c r="L432" s="3"/>
@@ -14846,7 +14903,7 @@
       <c r="T432" s="3"/>
       <c r="U432" s="5"/>
     </row>
-    <row r="433" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A433" s="12">
         <v>431</v>
       </c>
@@ -14863,7 +14920,9 @@
         <v>530</v>
       </c>
       <c r="H433" s="3"/>
-      <c r="I433" s="3"/>
+      <c r="I433" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J433" s="3"/>
       <c r="K433" s="3"/>
       <c r="L433" s="3"/>
@@ -14877,7 +14936,7 @@
       <c r="T433" s="3"/>
       <c r="U433" s="5"/>
     </row>
-    <row r="434" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A434" s="12">
         <v>432</v>
       </c>
@@ -14896,7 +14955,9 @@
         <v>519</v>
       </c>
       <c r="H434" s="3"/>
-      <c r="I434" s="3"/>
+      <c r="I434" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J434" s="3"/>
       <c r="K434" s="3"/>
       <c r="L434" s="3"/>
@@ -14910,7 +14971,7 @@
       <c r="T434" s="3"/>
       <c r="U434" s="5"/>
     </row>
-    <row r="435" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A435" s="12">
         <v>433</v>
       </c>
@@ -14929,7 +14990,9 @@
         <v>531</v>
       </c>
       <c r="H435" s="3"/>
-      <c r="I435" s="3"/>
+      <c r="I435" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J435" s="3"/>
       <c r="K435" s="3"/>
       <c r="L435" s="3"/>
@@ -15554,7 +15617,7 @@
       <c r="T454" s="3"/>
       <c r="U454" s="5"/>
     </row>
-    <row r="455" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A455" s="12">
         <v>453</v>
       </c>
@@ -15585,7 +15648,7 @@
       <c r="T455" s="3"/>
       <c r="U455" s="5"/>
     </row>
-    <row r="456" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A456" s="12">
         <v>454</v>
       </c>
@@ -15602,7 +15665,9 @@
         <v>530</v>
       </c>
       <c r="H456" s="3"/>
-      <c r="I456" s="3"/>
+      <c r="I456" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J456" s="3"/>
       <c r="K456" s="3"/>
       <c r="L456" s="3"/>
@@ -15616,7 +15681,7 @@
       <c r="T456" s="3"/>
       <c r="U456" s="5"/>
     </row>
-    <row r="457" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A457" s="12">
         <v>455</v>
       </c>
@@ -15635,7 +15700,9 @@
         <v>519</v>
       </c>
       <c r="H457" s="3"/>
-      <c r="I457" s="3"/>
+      <c r="I457" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J457" s="3"/>
       <c r="K457" s="3"/>
       <c r="L457" s="3"/>
@@ -15649,7 +15716,7 @@
       <c r="T457" s="3"/>
       <c r="U457" s="5"/>
     </row>
-    <row r="458" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A458" s="12">
         <v>456</v>
       </c>
@@ -15668,7 +15735,9 @@
         <v>532</v>
       </c>
       <c r="H458" s="3"/>
-      <c r="I458" s="3"/>
+      <c r="I458" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J458" s="3"/>
       <c r="K458" s="3"/>
       <c r="L458" s="3"/>
@@ -15682,7 +15751,7 @@
       <c r="T458" s="3"/>
       <c r="U458" s="5"/>
     </row>
-    <row r="459" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A459" s="12">
         <v>457</v>
       </c>
@@ -15715,7 +15784,7 @@
       <c r="T459" s="3"/>
       <c r="U459" s="5"/>
     </row>
-    <row r="460" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A460" s="12">
         <v>458</v>
       </c>
@@ -15732,7 +15801,9 @@
         <v>530</v>
       </c>
       <c r="H460" s="3"/>
-      <c r="I460" s="3"/>
+      <c r="I460" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J460" s="3"/>
       <c r="K460" s="3"/>
       <c r="L460" s="3"/>
@@ -15746,7 +15817,7 @@
       <c r="T460" s="3"/>
       <c r="U460" s="5"/>
     </row>
-    <row r="461" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A461" s="12">
         <v>459</v>
       </c>
@@ -15763,7 +15834,9 @@
         <v>530</v>
       </c>
       <c r="H461" s="3"/>
-      <c r="I461" s="3"/>
+      <c r="I461" s="28" t="s">
+        <v>537</v>
+      </c>
       <c r="J461" s="3"/>
       <c r="K461" s="3"/>
       <c r="L461" s="3"/>
@@ -18786,7 +18859,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="566" spans="1:21" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A566" s="12">
         <v>564</v>
       </c>
@@ -18804,6 +18877,9 @@
       <c r="G566" s="23" t="s">
         <v>534</v>
       </c>
+      <c r="I566" s="28" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="567" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A567" s="13">
@@ -18824,7 +18900,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="568" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A568" s="12">
         <v>566</v>
       </c>
@@ -18858,6 +18934,9 @@
       </c>
       <c r="G569" s="23" t="s">
         <v>534</v>
+      </c>
+      <c r="I569" s="28" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="570" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
https://jira.jda.com/browse/LRR-3315 wrong SOQ due to LT in start of LTP region 9 cases --50225,50227,50241,50242,50245,50246,50247,50487,50488
</commit_message>
<xml_diff>
--- a/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
+++ b/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\baseline\outputbaselines\1.TestCaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDA20F5-B153-4926-A511-87E115AB8B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE798D60-A1F6-4A89-B61A-B2FB157C853C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="544">
   <si>
     <t>S.No.</t>
   </si>
@@ -1677,6 +1677,18 @@
   </si>
   <si>
     <t>Trimming changes</t>
+  </si>
+  <si>
+    <t>Results better and projAvail not excessive</t>
+  </si>
+  <si>
+    <t>why not 25/25, earlier 2 weeks have that why not for 3rd week</t>
+  </si>
+  <si>
+    <t>Projavail better, but ratio off</t>
+  </si>
+  <si>
+    <t>no change in utility</t>
   </si>
 </sst>
 </file>
@@ -1892,7 +1904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1961,6 +1973,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2279,10 +2294,10 @@
   <dimension ref="A1:U576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="J463" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="K493" sqref="K493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2340,9 @@
       <c r="J1" s="14" t="s">
         <v>538</v>
       </c>
-      <c r="K1" s="14"/>
+      <c r="K1" s="16">
+        <v>44468</v>
+      </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
@@ -15474,7 +15491,9 @@
       <c r="J424" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K424" s="3"/>
+      <c r="K424" s="3" t="s">
+        <v>540</v>
+      </c>
       <c r="L424" s="3"/>
       <c r="M424" s="3"/>
       <c r="N424" s="3"/>
@@ -15544,7 +15563,9 @@
       <c r="J426" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K426" s="3"/>
+      <c r="K426" s="29" t="s">
+        <v>541</v>
+      </c>
       <c r="L426" s="3"/>
       <c r="M426" s="3"/>
       <c r="N426" s="3"/>
@@ -16586,7 +16607,9 @@
       <c r="J456" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K456" s="3"/>
+      <c r="K456" s="3" t="s">
+        <v>540</v>
+      </c>
       <c r="L456" s="3"/>
       <c r="M456" s="3"/>
       <c r="N456" s="3"/>
@@ -16623,7 +16646,9 @@
       <c r="J457" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K457" s="3"/>
+      <c r="K457" s="29" t="s">
+        <v>542</v>
+      </c>
       <c r="L457" s="3"/>
       <c r="M457" s="3"/>
       <c r="N457" s="3"/>
@@ -16730,7 +16755,9 @@
       <c r="J460" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K460" s="3"/>
+      <c r="K460" s="3" t="s">
+        <v>540</v>
+      </c>
       <c r="L460" s="3"/>
       <c r="M460" s="3"/>
       <c r="N460" s="3"/>
@@ -16765,7 +16792,9 @@
       <c r="J461" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K461" s="3"/>
+      <c r="K461" s="3" t="s">
+        <v>540</v>
+      </c>
       <c r="L461" s="3"/>
       <c r="M461" s="3"/>
       <c r="N461" s="3"/>
@@ -16798,7 +16827,9 @@
       <c r="J462" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K462" s="3"/>
+      <c r="K462" s="3" t="s">
+        <v>540</v>
+      </c>
       <c r="L462" s="3"/>
       <c r="M462" s="3"/>
       <c r="N462" s="3"/>
@@ -17701,7 +17732,7 @@
       <c r="T490" s="3"/>
       <c r="U490" s="5"/>
     </row>
-    <row r="491" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A491" s="12">
         <v>489</v>
       </c>
@@ -17732,7 +17763,7 @@
       <c r="T491" s="3"/>
       <c r="U491" s="5"/>
     </row>
-    <row r="492" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A492" s="12">
         <v>490</v>
       </c>
@@ -17751,7 +17782,9 @@
       <c r="J492" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="K492" s="3"/>
+      <c r="K492" s="24" t="s">
+        <v>543</v>
+      </c>
       <c r="L492" s="3"/>
       <c r="M492" s="3"/>
       <c r="N492" s="3"/>
@@ -17763,7 +17796,7 @@
       <c r="T492" s="3"/>
       <c r="U492" s="5"/>
     </row>
-    <row r="493" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A493" s="12">
         <v>491</v>
       </c>
@@ -17782,7 +17815,9 @@
       <c r="J493" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="K493" s="3"/>
+      <c r="K493" s="24" t="s">
+        <v>543</v>
+      </c>
       <c r="L493" s="3"/>
       <c r="M493" s="3"/>
       <c r="N493" s="3"/>

</xml_diff>

<commit_message>
https://jira.jda.com/browse/LRR-3797 case 50101 updated with min=55 and multiple=2 for item=5001. also updated excel with details.
</commit_message>
<xml_diff>
--- a/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
+++ b/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\baseline\outputbaselines\1.TestCaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6B9A0-675A-4AB9-B294-9C135BFF7A99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E966C9AB-6EB6-4640-999C-22A2A9A1A50C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="549">
   <si>
     <t>S.No.</t>
   </si>
@@ -1704,6 +1704,9 @@
   </si>
   <si>
     <t>changes due to Buy guide changes for Loblaws; wont order if not in buy guide</t>
+  </si>
+  <si>
+    <t>updated Min/Multiple qty for item=5001</t>
   </si>
 </sst>
 </file>
@@ -2477,14 +2480,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A5B6F5-D95C-4060-89B9-FDDC3DEF8E41}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C384" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D479" sqref="D479"/>
+      <selection pane="bottomRight" activeCell="F391" sqref="F391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,8 +2538,12 @@
       <c r="M1" s="16">
         <v>44479</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="N1" s="16">
+        <v>44508</v>
+      </c>
+      <c r="O1" s="16">
+        <v>44510</v>
+      </c>
       <c r="P1" s="14"/>
       <c r="Q1" s="14"/>
       <c r="R1" s="14"/>
@@ -2545,7 +2551,7 @@
       <c r="T1" s="14"/>
       <c r="U1" s="15"/>
     </row>
-    <row r="2" spans="1:21" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="29"/>
       <c r="C2" s="10"/>
@@ -2568,7 +2574,7 @@
       <c r="T2" s="10"/>
       <c r="U2" s="11"/>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2600,7 +2606,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -2632,7 +2638,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="5"/>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -2664,7 +2670,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="5"/>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -2696,7 +2702,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -2728,7 +2734,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="5"/>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -2760,7 +2766,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -2792,7 +2798,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -2824,7 +2830,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -2856,7 +2862,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -2888,7 +2894,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -2920,7 +2926,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>12</v>
       </c>
@@ -2952,7 +2958,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -2984,7 +2990,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="5"/>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>14</v>
       </c>
@@ -3016,7 +3022,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="5"/>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -3048,7 +3054,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -3080,7 +3086,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -3112,7 +3118,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -3144,7 +3150,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="5"/>
     </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -3176,7 +3182,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="5"/>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -3208,7 +3214,7 @@
       <c r="T22" s="3"/>
       <c r="U22" s="5"/>
     </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -3240,7 +3246,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="5"/>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -3272,7 +3278,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -3304,7 +3310,7 @@
       <c r="T25" s="3"/>
       <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -3336,7 +3342,7 @@
       <c r="T26" s="3"/>
       <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>25</v>
       </c>
@@ -3368,7 +3374,7 @@
       <c r="T27" s="3"/>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>26</v>
       </c>
@@ -3400,7 +3406,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="5"/>
     </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>27</v>
       </c>
@@ -3432,7 +3438,7 @@
       <c r="T29" s="3"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>28</v>
       </c>
@@ -3464,7 +3470,7 @@
       <c r="T30" s="3"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>29</v>
       </c>
@@ -3496,7 +3502,7 @@
       <c r="T31" s="3"/>
       <c r="U31" s="5"/>
     </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>30</v>
       </c>
@@ -3528,7 +3534,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>31</v>
       </c>
@@ -3560,7 +3566,7 @@
       <c r="T33" s="3"/>
       <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>32</v>
       </c>
@@ -3592,7 +3598,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="5"/>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>33</v>
       </c>
@@ -3624,7 +3630,7 @@
       <c r="T35" s="3"/>
       <c r="U35" s="5"/>
     </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>34</v>
       </c>
@@ -3656,7 +3662,7 @@
       <c r="T36" s="3"/>
       <c r="U36" s="5"/>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>35</v>
       </c>
@@ -3688,7 +3694,7 @@
       <c r="T37" s="3"/>
       <c r="U37" s="5"/>
     </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>36</v>
       </c>
@@ -3720,7 +3726,7 @@
       <c r="T38" s="3"/>
       <c r="U38" s="5"/>
     </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>37</v>
       </c>
@@ -3752,7 +3758,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="5"/>
     </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>38</v>
       </c>
@@ -3784,7 +3790,7 @@
       <c r="T40" s="3"/>
       <c r="U40" s="5"/>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>39</v>
       </c>
@@ -3816,7 +3822,7 @@
       <c r="T41" s="3"/>
       <c r="U41" s="5"/>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>40</v>
       </c>
@@ -3848,7 +3854,7 @@
       <c r="T42" s="3"/>
       <c r="U42" s="5"/>
     </row>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>41</v>
       </c>
@@ -3880,7 +3886,7 @@
       <c r="T43" s="3"/>
       <c r="U43" s="5"/>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>42</v>
       </c>
@@ -3912,7 +3918,7 @@
       <c r="T44" s="3"/>
       <c r="U44" s="5"/>
     </row>
-    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>43</v>
       </c>
@@ -3944,7 +3950,7 @@
       <c r="T45" s="3"/>
       <c r="U45" s="5"/>
     </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>44</v>
       </c>
@@ -3976,7 +3982,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="5"/>
     </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>45</v>
       </c>
@@ -4008,7 +4014,7 @@
       <c r="T47" s="3"/>
       <c r="U47" s="5"/>
     </row>
-    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>46</v>
       </c>
@@ -4040,7 +4046,7 @@
       <c r="T48" s="3"/>
       <c r="U48" s="5"/>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>47</v>
       </c>
@@ -4072,7 +4078,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="5"/>
     </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>48</v>
       </c>
@@ -4104,7 +4110,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="5"/>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>49</v>
       </c>
@@ -4136,7 +4142,7 @@
       <c r="T51" s="3"/>
       <c r="U51" s="5"/>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>50</v>
       </c>
@@ -4168,7 +4174,7 @@
       <c r="T52" s="3"/>
       <c r="U52" s="5"/>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>51</v>
       </c>
@@ -4200,7 +4206,7 @@
       <c r="T53" s="3"/>
       <c r="U53" s="5"/>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>52</v>
       </c>
@@ -4232,7 +4238,7 @@
       <c r="T54" s="3"/>
       <c r="U54" s="5"/>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>53</v>
       </c>
@@ -4264,7 +4270,7 @@
       <c r="T55" s="3"/>
       <c r="U55" s="5"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>54</v>
       </c>
@@ -4295,7 +4301,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="5"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>55</v>
       </c>
@@ -4327,7 +4333,7 @@
       <c r="T57" s="3"/>
       <c r="U57" s="5"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>56</v>
       </c>
@@ -4359,7 +4365,7 @@
       <c r="T58" s="3"/>
       <c r="U58" s="5"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>57</v>
       </c>
@@ -4391,7 +4397,7 @@
       <c r="T59" s="3"/>
       <c r="U59" s="5"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>58</v>
       </c>
@@ -4423,7 +4429,7 @@
       <c r="T60" s="3"/>
       <c r="U60" s="5"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>59</v>
       </c>
@@ -4455,7 +4461,7 @@
       <c r="T61" s="3"/>
       <c r="U61" s="5"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>60</v>
       </c>
@@ -4487,7 +4493,7 @@
       <c r="T62" s="3"/>
       <c r="U62" s="5"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>61</v>
       </c>
@@ -4519,7 +4525,7 @@
       <c r="T63" s="3"/>
       <c r="U63" s="5"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>62</v>
       </c>
@@ -4551,7 +4557,7 @@
       <c r="T64" s="3"/>
       <c r="U64" s="5"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>63</v>
       </c>
@@ -4583,7 +4589,7 @@
       <c r="T65" s="3"/>
       <c r="U65" s="5"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>64</v>
       </c>
@@ -4615,7 +4621,7 @@
       <c r="T66" s="3"/>
       <c r="U66" s="5"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>65</v>
       </c>
@@ -4647,7 +4653,7 @@
       <c r="T67" s="3"/>
       <c r="U67" s="5"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>66</v>
       </c>
@@ -4679,7 +4685,7 @@
       <c r="T68" s="3"/>
       <c r="U68" s="5"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>67</v>
       </c>
@@ -4711,7 +4717,7 @@
       <c r="T69" s="3"/>
       <c r="U69" s="5"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>68</v>
       </c>
@@ -4743,7 +4749,7 @@
       <c r="T70" s="3"/>
       <c r="U70" s="5"/>
     </row>
-    <row r="71" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>69</v>
       </c>
@@ -4775,7 +4781,7 @@
       <c r="T71" s="3"/>
       <c r="U71" s="5"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
         <v>70</v>
       </c>
@@ -4807,7 +4813,7 @@
       <c r="T72" s="3"/>
       <c r="U72" s="5"/>
     </row>
-    <row r="73" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="12">
         <v>71</v>
       </c>
@@ -4839,7 +4845,7 @@
       <c r="T73" s="3"/>
       <c r="U73" s="5"/>
     </row>
-    <row r="74" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>72</v>
       </c>
@@ -4871,7 +4877,7 @@
       <c r="T74" s="3"/>
       <c r="U74" s="5"/>
     </row>
-    <row r="75" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>73</v>
       </c>
@@ -4903,7 +4909,7 @@
       <c r="T75" s="3"/>
       <c r="U75" s="5"/>
     </row>
-    <row r="76" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>74</v>
       </c>
@@ -4935,7 +4941,7 @@
       <c r="T76" s="3"/>
       <c r="U76" s="5"/>
     </row>
-    <row r="77" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>75</v>
       </c>
@@ -4967,7 +4973,7 @@
       <c r="T77" s="3"/>
       <c r="U77" s="5"/>
     </row>
-    <row r="78" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>76</v>
       </c>
@@ -4999,7 +5005,7 @@
       <c r="T78" s="3"/>
       <c r="U78" s="5"/>
     </row>
-    <row r="79" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>77</v>
       </c>
@@ -5031,7 +5037,7 @@
       <c r="T79" s="3"/>
       <c r="U79" s="5"/>
     </row>
-    <row r="80" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>78</v>
       </c>
@@ -5063,7 +5069,7 @@
       <c r="T80" s="3"/>
       <c r="U80" s="5"/>
     </row>
-    <row r="81" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
         <v>79</v>
       </c>
@@ -5095,7 +5101,7 @@
       <c r="T81" s="3"/>
       <c r="U81" s="5"/>
     </row>
-    <row r="82" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>80</v>
       </c>
@@ -5127,7 +5133,7 @@
       <c r="T82" s="3"/>
       <c r="U82" s="5"/>
     </row>
-    <row r="83" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
         <v>81</v>
       </c>
@@ -5159,7 +5165,7 @@
       <c r="T83" s="3"/>
       <c r="U83" s="5"/>
     </row>
-    <row r="84" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>82</v>
       </c>
@@ -5191,7 +5197,7 @@
       <c r="T84" s="3"/>
       <c r="U84" s="5"/>
     </row>
-    <row r="85" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
         <v>83</v>
       </c>
@@ -5223,7 +5229,7 @@
       <c r="T85" s="3"/>
       <c r="U85" s="5"/>
     </row>
-    <row r="86" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
         <v>84</v>
       </c>
@@ -5255,7 +5261,7 @@
       <c r="T86" s="3"/>
       <c r="U86" s="5"/>
     </row>
-    <row r="87" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
         <v>85</v>
       </c>
@@ -5287,7 +5293,7 @@
       <c r="T87" s="3"/>
       <c r="U87" s="5"/>
     </row>
-    <row r="88" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="12">
         <v>86</v>
       </c>
@@ -5319,7 +5325,7 @@
       <c r="T88" s="3"/>
       <c r="U88" s="5"/>
     </row>
-    <row r="89" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="12">
         <v>87</v>
       </c>
@@ -5351,7 +5357,7 @@
       <c r="T89" s="3"/>
       <c r="U89" s="5"/>
     </row>
-    <row r="90" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
         <v>88</v>
       </c>
@@ -5383,7 +5389,7 @@
       <c r="T90" s="3"/>
       <c r="U90" s="5"/>
     </row>
-    <row r="91" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>89</v>
       </c>
@@ -5415,7 +5421,7 @@
       <c r="T91" s="3"/>
       <c r="U91" s="5"/>
     </row>
-    <row r="92" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>90</v>
       </c>
@@ -5449,7 +5455,7 @@
       <c r="T92" s="3"/>
       <c r="U92" s="5"/>
     </row>
-    <row r="93" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>91</v>
       </c>
@@ -5483,7 +5489,7 @@
       <c r="T93" s="3"/>
       <c r="U93" s="5"/>
     </row>
-    <row r="94" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>92</v>
       </c>
@@ -5515,7 +5521,7 @@
       <c r="T94" s="3"/>
       <c r="U94" s="5"/>
     </row>
-    <row r="95" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>93</v>
       </c>
@@ -5549,7 +5555,7 @@
       <c r="T95" s="3"/>
       <c r="U95" s="5"/>
     </row>
-    <row r="96" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12">
         <v>94</v>
       </c>
@@ -5583,7 +5589,7 @@
       <c r="T96" s="3"/>
       <c r="U96" s="5"/>
     </row>
-    <row r="97" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="12">
         <v>95</v>
       </c>
@@ -5615,7 +5621,7 @@
       <c r="T97" s="3"/>
       <c r="U97" s="5"/>
     </row>
-    <row r="98" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="12">
         <v>96</v>
       </c>
@@ -5647,7 +5653,7 @@
       <c r="T98" s="3"/>
       <c r="U98" s="5"/>
     </row>
-    <row r="99" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="12">
         <v>97</v>
       </c>
@@ -5679,7 +5685,7 @@
       <c r="T99" s="3"/>
       <c r="U99" s="5"/>
     </row>
-    <row r="100" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="12">
         <v>98</v>
       </c>
@@ -5711,7 +5717,7 @@
       <c r="T100" s="3"/>
       <c r="U100" s="5"/>
     </row>
-    <row r="101" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="12">
         <v>99</v>
       </c>
@@ -5743,7 +5749,7 @@
       <c r="T101" s="3"/>
       <c r="U101" s="5"/>
     </row>
-    <row r="102" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>100</v>
       </c>
@@ -5775,7 +5781,7 @@
       <c r="T102" s="3"/>
       <c r="U102" s="5"/>
     </row>
-    <row r="103" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="12">
         <v>101</v>
       </c>
@@ -5807,7 +5813,7 @@
       <c r="T103" s="3"/>
       <c r="U103" s="5"/>
     </row>
-    <row r="104" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="12">
         <v>102</v>
       </c>
@@ -5839,7 +5845,7 @@
       <c r="T104" s="3"/>
       <c r="U104" s="5"/>
     </row>
-    <row r="105" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="12">
         <v>103</v>
       </c>
@@ -5871,7 +5877,7 @@
       <c r="T105" s="3"/>
       <c r="U105" s="5"/>
     </row>
-    <row r="106" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="12">
         <v>104</v>
       </c>
@@ -5903,7 +5909,7 @@
       <c r="T106" s="3"/>
       <c r="U106" s="5"/>
     </row>
-    <row r="107" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="12">
         <v>105</v>
       </c>
@@ -5935,7 +5941,7 @@
       <c r="T107" s="3"/>
       <c r="U107" s="5"/>
     </row>
-    <row r="108" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="12">
         <v>106</v>
       </c>
@@ -5967,7 +5973,7 @@
       <c r="T108" s="3"/>
       <c r="U108" s="5"/>
     </row>
-    <row r="109" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="12">
         <v>107</v>
       </c>
@@ -5999,7 +6005,7 @@
       <c r="T109" s="3"/>
       <c r="U109" s="5"/>
     </row>
-    <row r="110" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="12">
         <v>108</v>
       </c>
@@ -6031,7 +6037,7 @@
       <c r="T110" s="3"/>
       <c r="U110" s="5"/>
     </row>
-    <row r="111" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="12">
         <v>109</v>
       </c>
@@ -6063,7 +6069,7 @@
       <c r="T111" s="3"/>
       <c r="U111" s="5"/>
     </row>
-    <row r="112" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="12">
         <v>110</v>
       </c>
@@ -6095,7 +6101,7 @@
       <c r="T112" s="3"/>
       <c r="U112" s="5"/>
     </row>
-    <row r="113" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="12">
         <v>111</v>
       </c>
@@ -6127,7 +6133,7 @@
       <c r="T113" s="3"/>
       <c r="U113" s="5"/>
     </row>
-    <row r="114" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="12">
         <v>112</v>
       </c>
@@ -6159,7 +6165,7 @@
       <c r="T114" s="3"/>
       <c r="U114" s="5"/>
     </row>
-    <row r="115" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="12">
         <v>113</v>
       </c>
@@ -6191,7 +6197,7 @@
       <c r="T115" s="3"/>
       <c r="U115" s="5"/>
     </row>
-    <row r="116" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="12">
         <v>114</v>
       </c>
@@ -6223,7 +6229,7 @@
       <c r="T116" s="3"/>
       <c r="U116" s="5"/>
     </row>
-    <row r="117" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="12">
         <v>115</v>
       </c>
@@ -6255,7 +6261,7 @@
       <c r="T117" s="3"/>
       <c r="U117" s="5"/>
     </row>
-    <row r="118" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="12">
         <v>116</v>
       </c>
@@ -6287,7 +6293,7 @@
       <c r="T118" s="3"/>
       <c r="U118" s="5"/>
     </row>
-    <row r="119" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="12">
         <v>117</v>
       </c>
@@ -6319,7 +6325,7 @@
       <c r="T119" s="3"/>
       <c r="U119" s="5"/>
     </row>
-    <row r="120" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="12">
         <v>118</v>
       </c>
@@ -6351,7 +6357,7 @@
       <c r="T120" s="3"/>
       <c r="U120" s="5"/>
     </row>
-    <row r="121" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="12">
         <v>119</v>
       </c>
@@ -6383,7 +6389,7 @@
       <c r="T121" s="3"/>
       <c r="U121" s="5"/>
     </row>
-    <row r="122" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" s="12">
         <v>120</v>
       </c>
@@ -6415,7 +6421,7 @@
       <c r="T122" s="3"/>
       <c r="U122" s="5"/>
     </row>
-    <row r="123" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="12">
         <v>121</v>
       </c>
@@ -6447,7 +6453,7 @@
       <c r="T123" s="3"/>
       <c r="U123" s="5"/>
     </row>
-    <row r="124" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12">
         <v>122</v>
       </c>
@@ -6481,7 +6487,7 @@
       <c r="T124" s="3"/>
       <c r="U124" s="5"/>
     </row>
-    <row r="125" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" s="12">
         <v>123</v>
       </c>
@@ -6513,7 +6519,7 @@
       <c r="T125" s="3"/>
       <c r="U125" s="5"/>
     </row>
-    <row r="126" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="12">
         <v>124</v>
       </c>
@@ -6545,7 +6551,7 @@
       <c r="T126" s="3"/>
       <c r="U126" s="5"/>
     </row>
-    <row r="127" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" s="12">
         <v>125</v>
       </c>
@@ -6577,7 +6583,7 @@
       <c r="T127" s="3"/>
       <c r="U127" s="5"/>
     </row>
-    <row r="128" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128" s="12">
         <v>126</v>
       </c>
@@ -6609,7 +6615,7 @@
       <c r="T128" s="3"/>
       <c r="U128" s="5"/>
     </row>
-    <row r="129" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" s="12">
         <v>127</v>
       </c>
@@ -6641,7 +6647,7 @@
       <c r="T129" s="3"/>
       <c r="U129" s="5"/>
     </row>
-    <row r="130" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130" s="12">
         <v>128</v>
       </c>
@@ -6673,7 +6679,7 @@
       <c r="T130" s="3"/>
       <c r="U130" s="5"/>
     </row>
-    <row r="131" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131" s="12">
         <v>129</v>
       </c>
@@ -6705,7 +6711,7 @@
       <c r="T131" s="3"/>
       <c r="U131" s="5"/>
     </row>
-    <row r="132" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132" s="12">
         <v>130</v>
       </c>
@@ -6737,7 +6743,7 @@
       <c r="T132" s="3"/>
       <c r="U132" s="5"/>
     </row>
-    <row r="133" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133" s="12">
         <v>131</v>
       </c>
@@ -6769,7 +6775,7 @@
       <c r="T133" s="3"/>
       <c r="U133" s="5"/>
     </row>
-    <row r="134" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134" s="12">
         <v>132</v>
       </c>
@@ -6801,7 +6807,7 @@
       <c r="T134" s="3"/>
       <c r="U134" s="5"/>
     </row>
-    <row r="135" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135" s="12">
         <v>133</v>
       </c>
@@ -6833,7 +6839,7 @@
       <c r="T135" s="3"/>
       <c r="U135" s="5"/>
     </row>
-    <row r="136" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136" s="12">
         <v>134</v>
       </c>
@@ -6865,7 +6871,7 @@
       <c r="T136" s="3"/>
       <c r="U136" s="5"/>
     </row>
-    <row r="137" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137" s="12">
         <v>135</v>
       </c>
@@ -6897,7 +6903,7 @@
       <c r="T137" s="3"/>
       <c r="U137" s="5"/>
     </row>
-    <row r="138" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" s="12">
         <v>136</v>
       </c>
@@ -6929,7 +6935,7 @@
       <c r="T138" s="3"/>
       <c r="U138" s="5"/>
     </row>
-    <row r="139" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139" s="12">
         <v>137</v>
       </c>
@@ -6961,7 +6967,7 @@
       <c r="T139" s="3"/>
       <c r="U139" s="5"/>
     </row>
-    <row r="140" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140" s="12">
         <v>138</v>
       </c>
@@ -6993,7 +6999,7 @@
       <c r="T140" s="3"/>
       <c r="U140" s="5"/>
     </row>
-    <row r="141" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A141" s="12">
         <v>139</v>
       </c>
@@ -7025,7 +7031,7 @@
       <c r="T141" s="3"/>
       <c r="U141" s="5"/>
     </row>
-    <row r="142" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142" s="12">
         <v>140</v>
       </c>
@@ -7057,7 +7063,7 @@
       <c r="T142" s="3"/>
       <c r="U142" s="5"/>
     </row>
-    <row r="143" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143" s="12">
         <v>141</v>
       </c>
@@ -7089,7 +7095,7 @@
       <c r="T143" s="3"/>
       <c r="U143" s="5"/>
     </row>
-    <row r="144" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144" s="12">
         <v>142</v>
       </c>
@@ -7121,7 +7127,7 @@
       <c r="T144" s="3"/>
       <c r="U144" s="5"/>
     </row>
-    <row r="145" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" s="12">
         <v>143</v>
       </c>
@@ -7153,7 +7159,7 @@
       <c r="T145" s="3"/>
       <c r="U145" s="5"/>
     </row>
-    <row r="146" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146" s="12">
         <v>144</v>
       </c>
@@ -7185,7 +7191,7 @@
       <c r="T146" s="3"/>
       <c r="U146" s="5"/>
     </row>
-    <row r="147" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147" s="12">
         <v>145</v>
       </c>
@@ -7217,7 +7223,7 @@
       <c r="T147" s="3"/>
       <c r="U147" s="5"/>
     </row>
-    <row r="148" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A148" s="12">
         <v>146</v>
       </c>
@@ -7249,7 +7255,7 @@
       <c r="T148" s="3"/>
       <c r="U148" s="5"/>
     </row>
-    <row r="149" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" s="12">
         <v>147</v>
       </c>
@@ -7281,7 +7287,7 @@
       <c r="T149" s="3"/>
       <c r="U149" s="5"/>
     </row>
-    <row r="150" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" s="12">
         <v>148</v>
       </c>
@@ -7313,7 +7319,7 @@
       <c r="T150" s="3"/>
       <c r="U150" s="5"/>
     </row>
-    <row r="151" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" s="12">
         <v>149</v>
       </c>
@@ -7345,7 +7351,7 @@
       <c r="T151" s="3"/>
       <c r="U151" s="5"/>
     </row>
-    <row r="152" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" s="12">
         <v>150</v>
       </c>
@@ -7377,7 +7383,7 @@
       <c r="T152" s="3"/>
       <c r="U152" s="5"/>
     </row>
-    <row r="153" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153" s="12">
         <v>151</v>
       </c>
@@ -7409,7 +7415,7 @@
       <c r="T153" s="3"/>
       <c r="U153" s="5"/>
     </row>
-    <row r="154" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="12">
         <v>152</v>
       </c>
@@ -7441,7 +7447,7 @@
       <c r="T154" s="3"/>
       <c r="U154" s="5"/>
     </row>
-    <row r="155" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="12">
         <v>153</v>
       </c>
@@ -7473,7 +7479,7 @@
       <c r="T155" s="3"/>
       <c r="U155" s="5"/>
     </row>
-    <row r="156" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="12">
         <v>154</v>
       </c>
@@ -7505,7 +7511,7 @@
       <c r="T156" s="3"/>
       <c r="U156" s="5"/>
     </row>
-    <row r="157" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="12">
         <v>155</v>
       </c>
@@ -7537,7 +7543,7 @@
       <c r="T157" s="3"/>
       <c r="U157" s="5"/>
     </row>
-    <row r="158" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="12">
         <v>156</v>
       </c>
@@ -7569,7 +7575,7 @@
       <c r="T158" s="3"/>
       <c r="U158" s="5"/>
     </row>
-    <row r="159" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="12">
         <v>157</v>
       </c>
@@ -7601,7 +7607,7 @@
       <c r="T159" s="3"/>
       <c r="U159" s="5"/>
     </row>
-    <row r="160" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="12">
         <v>158</v>
       </c>
@@ -7633,7 +7639,7 @@
       <c r="T160" s="3"/>
       <c r="U160" s="5"/>
     </row>
-    <row r="161" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="12">
         <v>159</v>
       </c>
@@ -7665,7 +7671,7 @@
       <c r="T161" s="3"/>
       <c r="U161" s="5"/>
     </row>
-    <row r="162" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="12">
         <v>160</v>
       </c>
@@ -7697,7 +7703,7 @@
       <c r="T162" s="3"/>
       <c r="U162" s="5"/>
     </row>
-    <row r="163" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="12">
         <v>161</v>
       </c>
@@ -7729,7 +7735,7 @@
       <c r="T163" s="3"/>
       <c r="U163" s="5"/>
     </row>
-    <row r="164" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164" s="12">
         <v>162</v>
       </c>
@@ -7761,7 +7767,7 @@
       <c r="T164" s="3"/>
       <c r="U164" s="5"/>
     </row>
-    <row r="165" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" s="12">
         <v>163</v>
       </c>
@@ -7793,7 +7799,7 @@
       <c r="T165" s="3"/>
       <c r="U165" s="5"/>
     </row>
-    <row r="166" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="12">
         <v>164</v>
       </c>
@@ -7825,7 +7831,7 @@
       <c r="T166" s="3"/>
       <c r="U166" s="5"/>
     </row>
-    <row r="167" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" s="12">
         <v>165</v>
       </c>
@@ -7857,7 +7863,7 @@
       <c r="T167" s="3"/>
       <c r="U167" s="5"/>
     </row>
-    <row r="168" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="12">
         <v>166</v>
       </c>
@@ -7889,7 +7895,7 @@
       <c r="T168" s="3"/>
       <c r="U168" s="5"/>
     </row>
-    <row r="169" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="12">
         <v>167</v>
       </c>
@@ -7921,7 +7927,7 @@
       <c r="T169" s="3"/>
       <c r="U169" s="5"/>
     </row>
-    <row r="170" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" s="12">
         <v>168</v>
       </c>
@@ -7953,7 +7959,7 @@
       <c r="T170" s="3"/>
       <c r="U170" s="5"/>
     </row>
-    <row r="171" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="12">
         <v>169</v>
       </c>
@@ -7985,7 +7991,7 @@
       <c r="T171" s="3"/>
       <c r="U171" s="5"/>
     </row>
-    <row r="172" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="12">
         <v>170</v>
       </c>
@@ -8017,7 +8023,7 @@
       <c r="T172" s="3"/>
       <c r="U172" s="5"/>
     </row>
-    <row r="173" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" s="12">
         <v>171</v>
       </c>
@@ -8049,7 +8055,7 @@
       <c r="T173" s="3"/>
       <c r="U173" s="5"/>
     </row>
-    <row r="174" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="12">
         <v>172</v>
       </c>
@@ -8081,7 +8087,7 @@
       <c r="T174" s="3"/>
       <c r="U174" s="5"/>
     </row>
-    <row r="175" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="12">
         <v>173</v>
       </c>
@@ -8113,7 +8119,7 @@
       <c r="T175" s="3"/>
       <c r="U175" s="5"/>
     </row>
-    <row r="176" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="12">
         <v>174</v>
       </c>
@@ -8145,7 +8151,7 @@
       <c r="T176" s="3"/>
       <c r="U176" s="5"/>
     </row>
-    <row r="177" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="12">
         <v>175</v>
       </c>
@@ -8177,7 +8183,7 @@
       <c r="T177" s="3"/>
       <c r="U177" s="5"/>
     </row>
-    <row r="178" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="12">
         <v>176</v>
       </c>
@@ -8209,7 +8215,7 @@
       <c r="T178" s="3"/>
       <c r="U178" s="5"/>
     </row>
-    <row r="179" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="12">
         <v>177</v>
       </c>
@@ -8241,7 +8247,7 @@
       <c r="T179" s="3"/>
       <c r="U179" s="5"/>
     </row>
-    <row r="180" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="12">
         <v>178</v>
       </c>
@@ -8273,7 +8279,7 @@
       <c r="T180" s="3"/>
       <c r="U180" s="5"/>
     </row>
-    <row r="181" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" s="12">
         <v>179</v>
       </c>
@@ -8305,7 +8311,7 @@
       <c r="T181" s="3"/>
       <c r="U181" s="5"/>
     </row>
-    <row r="182" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="12">
         <v>180</v>
       </c>
@@ -8337,7 +8343,7 @@
       <c r="T182" s="3"/>
       <c r="U182" s="5"/>
     </row>
-    <row r="183" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" s="12">
         <v>181</v>
       </c>
@@ -8369,7 +8375,7 @@
       <c r="T183" s="3"/>
       <c r="U183" s="5"/>
     </row>
-    <row r="184" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="12">
         <v>182</v>
       </c>
@@ -8401,7 +8407,7 @@
       <c r="T184" s="3"/>
       <c r="U184" s="5"/>
     </row>
-    <row r="185" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" s="12">
         <v>183</v>
       </c>
@@ -8433,7 +8439,7 @@
       <c r="T185" s="3"/>
       <c r="U185" s="5"/>
     </row>
-    <row r="186" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186" s="12">
         <v>184</v>
       </c>
@@ -8465,7 +8471,7 @@
       <c r="T186" s="3"/>
       <c r="U186" s="5"/>
     </row>
-    <row r="187" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" s="12">
         <v>185</v>
       </c>
@@ -8497,7 +8503,7 @@
       <c r="T187" s="3"/>
       <c r="U187" s="5"/>
     </row>
-    <row r="188" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188" s="12">
         <v>186</v>
       </c>
@@ -8529,7 +8535,7 @@
       <c r="T188" s="3"/>
       <c r="U188" s="5"/>
     </row>
-    <row r="189" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" s="12">
         <v>187</v>
       </c>
@@ -8561,7 +8567,7 @@
       <c r="T189" s="3"/>
       <c r="U189" s="5"/>
     </row>
-    <row r="190" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" s="12">
         <v>188</v>
       </c>
@@ -8593,7 +8599,7 @@
       <c r="T190" s="3"/>
       <c r="U190" s="5"/>
     </row>
-    <row r="191" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" s="12">
         <v>189</v>
       </c>
@@ -8625,7 +8631,7 @@
       <c r="T191" s="3"/>
       <c r="U191" s="5"/>
     </row>
-    <row r="192" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" s="12">
         <v>190</v>
       </c>
@@ -8657,7 +8663,7 @@
       <c r="T192" s="3"/>
       <c r="U192" s="5"/>
     </row>
-    <row r="193" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" s="12">
         <v>191</v>
       </c>
@@ -8689,7 +8695,7 @@
       <c r="T193" s="3"/>
       <c r="U193" s="5"/>
     </row>
-    <row r="194" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" s="12">
         <v>192</v>
       </c>
@@ -8721,7 +8727,7 @@
       <c r="T194" s="3"/>
       <c r="U194" s="5"/>
     </row>
-    <row r="195" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" s="12">
         <v>193</v>
       </c>
@@ -8753,7 +8759,7 @@
       <c r="T195" s="3"/>
       <c r="U195" s="5"/>
     </row>
-    <row r="196" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A196" s="12">
         <v>194</v>
       </c>
@@ -8785,7 +8791,7 @@
       <c r="T196" s="3"/>
       <c r="U196" s="5"/>
     </row>
-    <row r="197" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197" s="12">
         <v>195</v>
       </c>
@@ -8817,7 +8823,7 @@
       <c r="T197" s="3"/>
       <c r="U197" s="5"/>
     </row>
-    <row r="198" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198" s="12">
         <v>196</v>
       </c>
@@ -8849,7 +8855,7 @@
       <c r="T198" s="3"/>
       <c r="U198" s="5"/>
     </row>
-    <row r="199" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A199" s="12">
         <v>197</v>
       </c>
@@ -8881,7 +8887,7 @@
       <c r="T199" s="3"/>
       <c r="U199" s="5"/>
     </row>
-    <row r="200" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A200" s="12">
         <v>198</v>
       </c>
@@ -8913,7 +8919,7 @@
       <c r="T200" s="3"/>
       <c r="U200" s="5"/>
     </row>
-    <row r="201" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A201" s="12">
         <v>199</v>
       </c>
@@ -8945,7 +8951,7 @@
       <c r="T201" s="3"/>
       <c r="U201" s="5"/>
     </row>
-    <row r="202" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A202" s="12">
         <v>200</v>
       </c>
@@ -8977,7 +8983,7 @@
       <c r="T202" s="3"/>
       <c r="U202" s="5"/>
     </row>
-    <row r="203" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A203" s="12">
         <v>201</v>
       </c>
@@ -9009,7 +9015,7 @@
       <c r="T203" s="3"/>
       <c r="U203" s="5"/>
     </row>
-    <row r="204" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A204" s="12">
         <v>202</v>
       </c>
@@ -9041,7 +9047,7 @@
       <c r="T204" s="3"/>
       <c r="U204" s="5"/>
     </row>
-    <row r="205" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A205" s="12">
         <v>203</v>
       </c>
@@ -9073,7 +9079,7 @@
       <c r="T205" s="3"/>
       <c r="U205" s="5"/>
     </row>
-    <row r="206" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A206" s="12">
         <v>204</v>
       </c>
@@ -9105,7 +9111,7 @@
       <c r="T206" s="3"/>
       <c r="U206" s="5"/>
     </row>
-    <row r="207" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A207" s="12">
         <v>205</v>
       </c>
@@ -9137,7 +9143,7 @@
       <c r="T207" s="3"/>
       <c r="U207" s="5"/>
     </row>
-    <row r="208" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A208" s="12">
         <v>206</v>
       </c>
@@ -9169,7 +9175,7 @@
       <c r="T208" s="3"/>
       <c r="U208" s="5"/>
     </row>
-    <row r="209" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A209" s="12">
         <v>207</v>
       </c>
@@ -9201,7 +9207,7 @@
       <c r="T209" s="3"/>
       <c r="U209" s="5"/>
     </row>
-    <row r="210" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A210" s="12">
         <v>208</v>
       </c>
@@ -9233,7 +9239,7 @@
       <c r="T210" s="3"/>
       <c r="U210" s="5"/>
     </row>
-    <row r="211" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="12">
         <v>209</v>
       </c>
@@ -9265,7 +9271,7 @@
       <c r="T211" s="3"/>
       <c r="U211" s="5"/>
     </row>
-    <row r="212" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" s="12">
         <v>210</v>
       </c>
@@ -9297,7 +9303,7 @@
       <c r="T212" s="3"/>
       <c r="U212" s="5"/>
     </row>
-    <row r="213" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="12">
         <v>211</v>
       </c>
@@ -9329,7 +9335,7 @@
       <c r="T213" s="3"/>
       <c r="U213" s="5"/>
     </row>
-    <row r="214" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="12">
         <v>212</v>
       </c>
@@ -9361,7 +9367,7 @@
       <c r="T214" s="3"/>
       <c r="U214" s="5"/>
     </row>
-    <row r="215" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="12">
         <v>213</v>
       </c>
@@ -9393,7 +9399,7 @@
       <c r="T215" s="3"/>
       <c r="U215" s="5"/>
     </row>
-    <row r="216" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="12">
         <v>214</v>
       </c>
@@ -9425,7 +9431,7 @@
       <c r="T216" s="3"/>
       <c r="U216" s="5"/>
     </row>
-    <row r="217" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="12">
         <v>215</v>
       </c>
@@ -9457,7 +9463,7 @@
       <c r="T217" s="3"/>
       <c r="U217" s="5"/>
     </row>
-    <row r="218" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="12">
         <v>216</v>
       </c>
@@ -9489,7 +9495,7 @@
       <c r="T218" s="3"/>
       <c r="U218" s="5"/>
     </row>
-    <row r="219" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="12">
         <v>217</v>
       </c>
@@ -9521,7 +9527,7 @@
       <c r="T219" s="3"/>
       <c r="U219" s="5"/>
     </row>
-    <row r="220" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="12">
         <v>218</v>
       </c>
@@ -9553,7 +9559,7 @@
       <c r="T220" s="3"/>
       <c r="U220" s="5"/>
     </row>
-    <row r="221" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="12">
         <v>219</v>
       </c>
@@ -9585,7 +9591,7 @@
       <c r="T221" s="3"/>
       <c r="U221" s="5"/>
     </row>
-    <row r="222" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="12">
         <v>220</v>
       </c>
@@ -9617,7 +9623,7 @@
       <c r="T222" s="3"/>
       <c r="U222" s="5"/>
     </row>
-    <row r="223" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="12">
         <v>221</v>
       </c>
@@ -9649,7 +9655,7 @@
       <c r="T223" s="3"/>
       <c r="U223" s="5"/>
     </row>
-    <row r="224" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="12">
         <v>222</v>
       </c>
@@ -9681,7 +9687,7 @@
       <c r="T224" s="3"/>
       <c r="U224" s="5"/>
     </row>
-    <row r="225" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="12">
         <v>223</v>
       </c>
@@ -9713,7 +9719,7 @@
       <c r="T225" s="3"/>
       <c r="U225" s="5"/>
     </row>
-    <row r="226" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="12">
         <v>224</v>
       </c>
@@ -9745,7 +9751,7 @@
       <c r="T226" s="3"/>
       <c r="U226" s="5"/>
     </row>
-    <row r="227" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="12">
         <v>225</v>
       </c>
@@ -9777,7 +9783,7 @@
       <c r="T227" s="3"/>
       <c r="U227" s="5"/>
     </row>
-    <row r="228" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="12">
         <v>226</v>
       </c>
@@ -9809,7 +9815,7 @@
       <c r="T228" s="3"/>
       <c r="U228" s="5"/>
     </row>
-    <row r="229" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" s="12">
         <v>227</v>
       </c>
@@ -9841,7 +9847,7 @@
       <c r="T229" s="3"/>
       <c r="U229" s="5"/>
     </row>
-    <row r="230" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="12">
         <v>228</v>
       </c>
@@ -9873,7 +9879,7 @@
       <c r="T230" s="3"/>
       <c r="U230" s="5"/>
     </row>
-    <row r="231" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="12">
         <v>229</v>
       </c>
@@ -9905,7 +9911,7 @@
       <c r="T231" s="3"/>
       <c r="U231" s="5"/>
     </row>
-    <row r="232" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="12">
         <v>230</v>
       </c>
@@ -9937,7 +9943,7 @@
       <c r="T232" s="3"/>
       <c r="U232" s="5"/>
     </row>
-    <row r="233" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A233" s="12">
         <v>231</v>
       </c>
@@ -9969,7 +9975,7 @@
       <c r="T233" s="3"/>
       <c r="U233" s="5"/>
     </row>
-    <row r="234" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="12">
         <v>232</v>
       </c>
@@ -10001,7 +10007,7 @@
       <c r="T234" s="3"/>
       <c r="U234" s="5"/>
     </row>
-    <row r="235" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="12">
         <v>233</v>
       </c>
@@ -10033,7 +10039,7 @@
       <c r="T235" s="3"/>
       <c r="U235" s="5"/>
     </row>
-    <row r="236" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A236" s="12">
         <v>234</v>
       </c>
@@ -10065,7 +10071,7 @@
       <c r="T236" s="3"/>
       <c r="U236" s="5"/>
     </row>
-    <row r="237" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237" s="12">
         <v>235</v>
       </c>
@@ -10097,7 +10103,7 @@
       <c r="T237" s="3"/>
       <c r="U237" s="5"/>
     </row>
-    <row r="238" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" s="12">
         <v>236</v>
       </c>
@@ -10129,7 +10135,7 @@
       <c r="T238" s="3"/>
       <c r="U238" s="5"/>
     </row>
-    <row r="239" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A239" s="12">
         <v>237</v>
       </c>
@@ -10161,7 +10167,7 @@
       <c r="T239" s="3"/>
       <c r="U239" s="5"/>
     </row>
-    <row r="240" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" s="12">
         <v>238</v>
       </c>
@@ -10193,7 +10199,7 @@
       <c r="T240" s="3"/>
       <c r="U240" s="5"/>
     </row>
-    <row r="241" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A241" s="12">
         <v>239</v>
       </c>
@@ -10225,7 +10231,7 @@
       <c r="T241" s="3"/>
       <c r="U241" s="5"/>
     </row>
-    <row r="242" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A242" s="12">
         <v>240</v>
       </c>
@@ -10257,7 +10263,7 @@
       <c r="T242" s="3"/>
       <c r="U242" s="5"/>
     </row>
-    <row r="243" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A243" s="12">
         <v>241</v>
       </c>
@@ -10289,7 +10295,7 @@
       <c r="T243" s="3"/>
       <c r="U243" s="5"/>
     </row>
-    <row r="244" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A244" s="12">
         <v>242</v>
       </c>
@@ -10321,7 +10327,7 @@
       <c r="T244" s="3"/>
       <c r="U244" s="5"/>
     </row>
-    <row r="245" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A245" s="12">
         <v>243</v>
       </c>
@@ -10353,7 +10359,7 @@
       <c r="T245" s="3"/>
       <c r="U245" s="5"/>
     </row>
-    <row r="246" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A246" s="12">
         <v>244</v>
       </c>
@@ -10385,7 +10391,7 @@
       <c r="T246" s="3"/>
       <c r="U246" s="5"/>
     </row>
-    <row r="247" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A247" s="12">
         <v>245</v>
       </c>
@@ -10417,7 +10423,7 @@
       <c r="T247" s="3"/>
       <c r="U247" s="5"/>
     </row>
-    <row r="248" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" s="12">
         <v>246</v>
       </c>
@@ -10449,7 +10455,7 @@
       <c r="T248" s="3"/>
       <c r="U248" s="5"/>
     </row>
-    <row r="249" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249" s="12">
         <v>247</v>
       </c>
@@ -10481,7 +10487,7 @@
       <c r="T249" s="3"/>
       <c r="U249" s="5"/>
     </row>
-    <row r="250" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250" s="12">
         <v>248</v>
       </c>
@@ -10513,7 +10519,7 @@
       <c r="T250" s="3"/>
       <c r="U250" s="5"/>
     </row>
-    <row r="251" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251" s="12">
         <v>249</v>
       </c>
@@ -10545,7 +10551,7 @@
       <c r="T251" s="3"/>
       <c r="U251" s="5"/>
     </row>
-    <row r="252" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252" s="12">
         <v>250</v>
       </c>
@@ -10577,7 +10583,7 @@
       <c r="T252" s="3"/>
       <c r="U252" s="5"/>
     </row>
-    <row r="253" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" s="12">
         <v>251</v>
       </c>
@@ -10609,7 +10615,7 @@
       <c r="T253" s="3"/>
       <c r="U253" s="5"/>
     </row>
-    <row r="254" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" s="12">
         <v>252</v>
       </c>
@@ -10641,7 +10647,7 @@
       <c r="T254" s="3"/>
       <c r="U254" s="5"/>
     </row>
-    <row r="255" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" s="12">
         <v>253</v>
       </c>
@@ -10673,7 +10679,7 @@
       <c r="T255" s="3"/>
       <c r="U255" s="5"/>
     </row>
-    <row r="256" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" s="12">
         <v>254</v>
       </c>
@@ -10705,7 +10711,7 @@
       <c r="T256" s="3"/>
       <c r="U256" s="5"/>
     </row>
-    <row r="257" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="12">
         <v>255</v>
       </c>
@@ -10737,7 +10743,7 @@
       <c r="T257" s="3"/>
       <c r="U257" s="5"/>
     </row>
-    <row r="258" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="12">
         <v>256</v>
       </c>
@@ -10769,7 +10775,7 @@
       <c r="T258" s="3"/>
       <c r="U258" s="5"/>
     </row>
-    <row r="259" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" s="12">
         <v>257</v>
       </c>
@@ -10801,7 +10807,7 @@
       <c r="T259" s="3"/>
       <c r="U259" s="5"/>
     </row>
-    <row r="260" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A260" s="12">
         <v>258</v>
       </c>
@@ -10833,7 +10839,7 @@
       <c r="T260" s="3"/>
       <c r="U260" s="5"/>
     </row>
-    <row r="261" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" s="12">
         <v>259</v>
       </c>
@@ -10865,7 +10871,7 @@
       <c r="T261" s="3"/>
       <c r="U261" s="5"/>
     </row>
-    <row r="262" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" s="12">
         <v>260</v>
       </c>
@@ -10897,7 +10903,7 @@
       <c r="T262" s="3"/>
       <c r="U262" s="5"/>
     </row>
-    <row r="263" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="12">
         <v>261</v>
       </c>
@@ -10929,7 +10935,7 @@
       <c r="T263" s="3"/>
       <c r="U263" s="5"/>
     </row>
-    <row r="264" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="12">
         <v>262</v>
       </c>
@@ -10961,7 +10967,7 @@
       <c r="T264" s="3"/>
       <c r="U264" s="5"/>
     </row>
-    <row r="265" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="12">
         <v>263</v>
       </c>
@@ -10993,7 +10999,7 @@
       <c r="T265" s="3"/>
       <c r="U265" s="5"/>
     </row>
-    <row r="266" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" s="12">
         <v>264</v>
       </c>
@@ -11025,7 +11031,7 @@
       <c r="T266" s="3"/>
       <c r="U266" s="5"/>
     </row>
-    <row r="267" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" s="12">
         <v>265</v>
       </c>
@@ -11057,7 +11063,7 @@
       <c r="T267" s="3"/>
       <c r="U267" s="5"/>
     </row>
-    <row r="268" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A268" s="12">
         <v>266</v>
       </c>
@@ -11089,7 +11095,7 @@
       <c r="T268" s="3"/>
       <c r="U268" s="5"/>
     </row>
-    <row r="269" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" s="12">
         <v>267</v>
       </c>
@@ -11121,7 +11127,7 @@
       <c r="T269" s="3"/>
       <c r="U269" s="5"/>
     </row>
-    <row r="270" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="12">
         <v>268</v>
       </c>
@@ -11153,7 +11159,7 @@
       <c r="T270" s="3"/>
       <c r="U270" s="5"/>
     </row>
-    <row r="271" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="12">
         <v>269</v>
       </c>
@@ -11185,7 +11191,7 @@
       <c r="T271" s="3"/>
       <c r="U271" s="5"/>
     </row>
-    <row r="272" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="12">
         <v>270</v>
       </c>
@@ -11217,7 +11223,7 @@
       <c r="T272" s="3"/>
       <c r="U272" s="5"/>
     </row>
-    <row r="273" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273" s="12">
         <v>271</v>
       </c>
@@ -11249,7 +11255,7 @@
       <c r="T273" s="3"/>
       <c r="U273" s="5"/>
     </row>
-    <row r="274" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A274" s="12">
         <v>272</v>
       </c>
@@ -11281,7 +11287,7 @@
       <c r="T274" s="3"/>
       <c r="U274" s="5"/>
     </row>
-    <row r="275" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A275" s="12">
         <v>273</v>
       </c>
@@ -11313,7 +11319,7 @@
       <c r="T275" s="3"/>
       <c r="U275" s="5"/>
     </row>
-    <row r="276" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A276" s="12">
         <v>274</v>
       </c>
@@ -11345,7 +11351,7 @@
       <c r="T276" s="3"/>
       <c r="U276" s="5"/>
     </row>
-    <row r="277" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A277" s="12">
         <v>275</v>
       </c>
@@ -11377,7 +11383,7 @@
       <c r="T277" s="3"/>
       <c r="U277" s="5"/>
     </row>
-    <row r="278" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="12">
         <v>276</v>
       </c>
@@ -11409,7 +11415,7 @@
       <c r="T278" s="3"/>
       <c r="U278" s="5"/>
     </row>
-    <row r="279" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A279" s="12">
         <v>277</v>
       </c>
@@ -11441,7 +11447,7 @@
       <c r="T279" s="3"/>
       <c r="U279" s="5"/>
     </row>
-    <row r="280" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A280" s="12">
         <v>278</v>
       </c>
@@ -11473,7 +11479,7 @@
       <c r="T280" s="3"/>
       <c r="U280" s="5"/>
     </row>
-    <row r="281" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" s="12">
         <v>279</v>
       </c>
@@ -11505,7 +11511,7 @@
       <c r="T281" s="3"/>
       <c r="U281" s="5"/>
     </row>
-    <row r="282" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="12">
         <v>280</v>
       </c>
@@ -11537,7 +11543,7 @@
       <c r="T282" s="3"/>
       <c r="U282" s="5"/>
     </row>
-    <row r="283" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A283" s="12">
         <v>281</v>
       </c>
@@ -11569,7 +11575,7 @@
       <c r="T283" s="3"/>
       <c r="U283" s="5"/>
     </row>
-    <row r="284" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A284" s="12">
         <v>282</v>
       </c>
@@ -11601,7 +11607,7 @@
       <c r="T284" s="3"/>
       <c r="U284" s="5"/>
     </row>
-    <row r="285" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A285" s="12">
         <v>283</v>
       </c>
@@ -11633,7 +11639,7 @@
       <c r="T285" s="3"/>
       <c r="U285" s="5"/>
     </row>
-    <row r="286" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A286" s="12">
         <v>284</v>
       </c>
@@ -11665,7 +11671,7 @@
       <c r="T286" s="3"/>
       <c r="U286" s="5"/>
     </row>
-    <row r="287" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A287" s="12">
         <v>285</v>
       </c>
@@ -11697,7 +11703,7 @@
       <c r="T287" s="3"/>
       <c r="U287" s="5"/>
     </row>
-    <row r="288" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A288" s="12">
         <v>286</v>
       </c>
@@ -11729,7 +11735,7 @@
       <c r="T288" s="3"/>
       <c r="U288" s="5"/>
     </row>
-    <row r="289" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A289" s="12">
         <v>287</v>
       </c>
@@ -11761,7 +11767,7 @@
       <c r="T289" s="3"/>
       <c r="U289" s="5"/>
     </row>
-    <row r="290" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" s="12">
         <v>288</v>
       </c>
@@ -11793,7 +11799,7 @@
       <c r="T290" s="3"/>
       <c r="U290" s="5"/>
     </row>
-    <row r="291" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" s="12">
         <v>289</v>
       </c>
@@ -11825,7 +11831,7 @@
       <c r="T291" s="3"/>
       <c r="U291" s="5"/>
     </row>
-    <row r="292" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A292" s="12">
         <v>290</v>
       </c>
@@ -11857,7 +11863,7 @@
       <c r="T292" s="3"/>
       <c r="U292" s="5"/>
     </row>
-    <row r="293" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A293" s="12">
         <v>291</v>
       </c>
@@ -11889,7 +11895,7 @@
       <c r="T293" s="3"/>
       <c r="U293" s="5"/>
     </row>
-    <row r="294" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A294" s="12">
         <v>292</v>
       </c>
@@ -11921,7 +11927,7 @@
       <c r="T294" s="3"/>
       <c r="U294" s="5"/>
     </row>
-    <row r="295" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A295" s="12">
         <v>293</v>
       </c>
@@ -11953,7 +11959,7 @@
       <c r="T295" s="3"/>
       <c r="U295" s="5"/>
     </row>
-    <row r="296" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" s="12">
         <v>294</v>
       </c>
@@ -11985,7 +11991,7 @@
       <c r="T296" s="3"/>
       <c r="U296" s="5"/>
     </row>
-    <row r="297" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" s="12">
         <v>295</v>
       </c>
@@ -12017,7 +12023,7 @@
       <c r="T297" s="3"/>
       <c r="U297" s="5"/>
     </row>
-    <row r="298" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" s="12">
         <v>296</v>
       </c>
@@ -12049,7 +12055,7 @@
       <c r="T298" s="3"/>
       <c r="U298" s="5"/>
     </row>
-    <row r="299" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" s="12">
         <v>297</v>
       </c>
@@ -12081,7 +12087,7 @@
       <c r="T299" s="3"/>
       <c r="U299" s="5"/>
     </row>
-    <row r="300" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A300" s="12">
         <v>298</v>
       </c>
@@ -12113,7 +12119,7 @@
       <c r="T300" s="3"/>
       <c r="U300" s="5"/>
     </row>
-    <row r="301" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A301" s="12">
         <v>299</v>
       </c>
@@ -12145,7 +12151,7 @@
       <c r="T301" s="3"/>
       <c r="U301" s="5"/>
     </row>
-    <row r="302" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" s="12">
         <v>300</v>
       </c>
@@ -12177,7 +12183,7 @@
       <c r="T302" s="3"/>
       <c r="U302" s="5"/>
     </row>
-    <row r="303" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" s="12">
         <v>301</v>
       </c>
@@ -12209,7 +12215,7 @@
       <c r="T303" s="3"/>
       <c r="U303" s="5"/>
     </row>
-    <row r="304" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" s="12">
         <v>302</v>
       </c>
@@ -12241,7 +12247,7 @@
       <c r="T304" s="3"/>
       <c r="U304" s="5"/>
     </row>
-    <row r="305" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="12">
         <v>303</v>
       </c>
@@ -12273,7 +12279,7 @@
       <c r="T305" s="3"/>
       <c r="U305" s="5"/>
     </row>
-    <row r="306" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A306" s="12">
         <v>304</v>
       </c>
@@ -12305,7 +12311,7 @@
       <c r="T306" s="3"/>
       <c r="U306" s="5"/>
     </row>
-    <row r="307" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A307" s="12">
         <v>305</v>
       </c>
@@ -12337,7 +12343,7 @@
       <c r="T307" s="3"/>
       <c r="U307" s="5"/>
     </row>
-    <row r="308" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A308" s="12">
         <v>306</v>
       </c>
@@ -12369,7 +12375,7 @@
       <c r="T308" s="3"/>
       <c r="U308" s="5"/>
     </row>
-    <row r="309" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" s="12">
         <v>307</v>
       </c>
@@ -12401,7 +12407,7 @@
       <c r="T309" s="3"/>
       <c r="U309" s="5"/>
     </row>
-    <row r="310" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="12">
         <v>308</v>
       </c>
@@ -12433,7 +12439,7 @@
       <c r="T310" s="3"/>
       <c r="U310" s="5"/>
     </row>
-    <row r="311" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A311" s="12">
         <v>309</v>
       </c>
@@ -12465,7 +12471,7 @@
       <c r="T311" s="3"/>
       <c r="U311" s="5"/>
     </row>
-    <row r="312" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A312" s="12">
         <v>310</v>
       </c>
@@ -12497,7 +12503,7 @@
       <c r="T312" s="3"/>
       <c r="U312" s="5"/>
     </row>
-    <row r="313" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A313" s="12">
         <v>311</v>
       </c>
@@ -12529,7 +12535,7 @@
       <c r="T313" s="3"/>
       <c r="U313" s="5"/>
     </row>
-    <row r="314" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A314" s="12">
         <v>312</v>
       </c>
@@ -12561,7 +12567,7 @@
       <c r="T314" s="3"/>
       <c r="U314" s="5"/>
     </row>
-    <row r="315" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A315" s="12">
         <v>313</v>
       </c>
@@ -12593,7 +12599,7 @@
       <c r="T315" s="3"/>
       <c r="U315" s="5"/>
     </row>
-    <row r="316" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A316" s="12">
         <v>314</v>
       </c>
@@ -12625,7 +12631,7 @@
       <c r="T316" s="3"/>
       <c r="U316" s="5"/>
     </row>
-    <row r="317" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A317" s="12">
         <v>315</v>
       </c>
@@ -12657,7 +12663,7 @@
       <c r="T317" s="3"/>
       <c r="U317" s="5"/>
     </row>
-    <row r="318" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A318" s="12">
         <v>316</v>
       </c>
@@ -12689,7 +12695,7 @@
       <c r="T318" s="3"/>
       <c r="U318" s="5"/>
     </row>
-    <row r="319" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A319" s="12">
         <v>317</v>
       </c>
@@ -12721,7 +12727,7 @@
       <c r="T319" s="3"/>
       <c r="U319" s="5"/>
     </row>
-    <row r="320" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A320" s="12">
         <v>318</v>
       </c>
@@ -12753,7 +12759,7 @@
       <c r="T320" s="3"/>
       <c r="U320" s="5"/>
     </row>
-    <row r="321" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A321" s="12">
         <v>319</v>
       </c>
@@ -12785,7 +12791,7 @@
       <c r="T321" s="3"/>
       <c r="U321" s="5"/>
     </row>
-    <row r="322" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A322" s="12">
         <v>320</v>
       </c>
@@ -12817,7 +12823,7 @@
       <c r="T322" s="3"/>
       <c r="U322" s="5"/>
     </row>
-    <row r="323" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A323" s="12">
         <v>321</v>
       </c>
@@ -12849,7 +12855,7 @@
       <c r="T323" s="3"/>
       <c r="U323" s="5"/>
     </row>
-    <row r="324" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A324" s="12">
         <v>322</v>
       </c>
@@ -12881,7 +12887,7 @@
       <c r="T324" s="3"/>
       <c r="U324" s="5"/>
     </row>
-    <row r="325" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A325" s="12">
         <v>323</v>
       </c>
@@ -12913,7 +12919,7 @@
       <c r="T325" s="3"/>
       <c r="U325" s="5"/>
     </row>
-    <row r="326" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A326" s="12">
         <v>324</v>
       </c>
@@ -12945,7 +12951,7 @@
       <c r="T326" s="3"/>
       <c r="U326" s="5"/>
     </row>
-    <row r="327" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A327" s="12">
         <v>325</v>
       </c>
@@ -12977,7 +12983,7 @@
       <c r="T327" s="3"/>
       <c r="U327" s="5"/>
     </row>
-    <row r="328" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A328" s="12">
         <v>326</v>
       </c>
@@ -13009,7 +13015,7 @@
       <c r="T328" s="3"/>
       <c r="U328" s="5"/>
     </row>
-    <row r="329" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A329" s="12">
         <v>327</v>
       </c>
@@ -13041,7 +13047,7 @@
       <c r="T329" s="3"/>
       <c r="U329" s="5"/>
     </row>
-    <row r="330" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A330" s="12">
         <v>328</v>
       </c>
@@ -13073,7 +13079,7 @@
       <c r="T330" s="3"/>
       <c r="U330" s="5"/>
     </row>
-    <row r="331" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A331" s="12">
         <v>329</v>
       </c>
@@ -13105,7 +13111,7 @@
       <c r="T331" s="3"/>
       <c r="U331" s="5"/>
     </row>
-    <row r="332" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A332" s="12">
         <v>330</v>
       </c>
@@ -13137,7 +13143,7 @@
       <c r="T332" s="3"/>
       <c r="U332" s="5"/>
     </row>
-    <row r="333" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A333" s="12">
         <v>331</v>
       </c>
@@ -13169,7 +13175,7 @@
       <c r="T333" s="3"/>
       <c r="U333" s="5"/>
     </row>
-    <row r="334" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A334" s="12">
         <v>332</v>
       </c>
@@ -13201,7 +13207,7 @@
       <c r="T334" s="3"/>
       <c r="U334" s="5"/>
     </row>
-    <row r="335" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A335" s="12">
         <v>333</v>
       </c>
@@ -13233,7 +13239,7 @@
       <c r="T335" s="3"/>
       <c r="U335" s="5"/>
     </row>
-    <row r="336" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A336" s="12">
         <v>334</v>
       </c>
@@ -13265,7 +13271,7 @@
       <c r="T336" s="3"/>
       <c r="U336" s="5"/>
     </row>
-    <row r="337" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A337" s="12">
         <v>335</v>
       </c>
@@ -13297,7 +13303,7 @@
       <c r="T337" s="3"/>
       <c r="U337" s="5"/>
     </row>
-    <row r="338" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A338" s="12">
         <v>336</v>
       </c>
@@ -13329,7 +13335,7 @@
       <c r="T338" s="3"/>
       <c r="U338" s="5"/>
     </row>
-    <row r="339" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A339" s="12">
         <v>337</v>
       </c>
@@ -13361,7 +13367,7 @@
       <c r="T339" s="3"/>
       <c r="U339" s="5"/>
     </row>
-    <row r="340" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A340" s="12">
         <v>338</v>
       </c>
@@ -13393,7 +13399,7 @@
       <c r="T340" s="3"/>
       <c r="U340" s="5"/>
     </row>
-    <row r="341" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A341" s="12">
         <v>339</v>
       </c>
@@ -13425,7 +13431,7 @@
       <c r="T341" s="3"/>
       <c r="U341" s="5"/>
     </row>
-    <row r="342" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A342" s="12">
         <v>340</v>
       </c>
@@ -13457,7 +13463,7 @@
       <c r="T342" s="3"/>
       <c r="U342" s="5"/>
     </row>
-    <row r="343" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A343" s="12">
         <v>341</v>
       </c>
@@ -13489,7 +13495,7 @@
       <c r="T343" s="3"/>
       <c r="U343" s="5"/>
     </row>
-    <row r="344" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A344" s="12">
         <v>342</v>
       </c>
@@ -13521,7 +13527,7 @@
       <c r="T344" s="3"/>
       <c r="U344" s="5"/>
     </row>
-    <row r="345" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A345" s="12">
         <v>343</v>
       </c>
@@ -13553,7 +13559,7 @@
       <c r="T345" s="3"/>
       <c r="U345" s="5"/>
     </row>
-    <row r="346" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A346" s="12">
         <v>344</v>
       </c>
@@ -13585,7 +13591,7 @@
       <c r="T346" s="3"/>
       <c r="U346" s="5"/>
     </row>
-    <row r="347" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A347" s="12">
         <v>345</v>
       </c>
@@ -13617,7 +13623,7 @@
       <c r="T347" s="3"/>
       <c r="U347" s="5"/>
     </row>
-    <row r="348" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A348" s="12">
         <v>346</v>
       </c>
@@ -13649,7 +13655,7 @@
       <c r="T348" s="3"/>
       <c r="U348" s="5"/>
     </row>
-    <row r="349" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A349" s="12">
         <v>347</v>
       </c>
@@ -13681,7 +13687,7 @@
       <c r="T349" s="3"/>
       <c r="U349" s="5"/>
     </row>
-    <row r="350" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A350" s="12">
         <v>348</v>
       </c>
@@ -13713,7 +13719,7 @@
       <c r="T350" s="3"/>
       <c r="U350" s="5"/>
     </row>
-    <row r="351" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A351" s="12">
         <v>349</v>
       </c>
@@ -13745,7 +13751,7 @@
       <c r="T351" s="3"/>
       <c r="U351" s="5"/>
     </row>
-    <row r="352" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A352" s="12">
         <v>350</v>
       </c>
@@ -13777,7 +13783,7 @@
       <c r="T352" s="3"/>
       <c r="U352" s="5"/>
     </row>
-    <row r="353" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A353" s="12">
         <v>351</v>
       </c>
@@ -13809,7 +13815,7 @@
       <c r="T353" s="3"/>
       <c r="U353" s="5"/>
     </row>
-    <row r="354" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A354" s="12">
         <v>352</v>
       </c>
@@ -13841,7 +13847,7 @@
       <c r="T354" s="3"/>
       <c r="U354" s="5"/>
     </row>
-    <row r="355" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A355" s="12">
         <v>353</v>
       </c>
@@ -13873,7 +13879,7 @@
       <c r="T355" s="3"/>
       <c r="U355" s="5"/>
     </row>
-    <row r="356" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A356" s="12">
         <v>354</v>
       </c>
@@ -13905,7 +13911,7 @@
       <c r="T356" s="3"/>
       <c r="U356" s="5"/>
     </row>
-    <row r="357" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A357" s="12">
         <v>355</v>
       </c>
@@ -13937,7 +13943,7 @@
       <c r="T357" s="3"/>
       <c r="U357" s="5"/>
     </row>
-    <row r="358" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A358" s="12">
         <v>356</v>
       </c>
@@ -13969,7 +13975,7 @@
       <c r="T358" s="3"/>
       <c r="U358" s="5"/>
     </row>
-    <row r="359" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A359" s="12">
         <v>357</v>
       </c>
@@ -14001,7 +14007,7 @@
       <c r="T359" s="3"/>
       <c r="U359" s="5"/>
     </row>
-    <row r="360" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A360" s="12">
         <v>358</v>
       </c>
@@ -14033,7 +14039,7 @@
       <c r="T360" s="3"/>
       <c r="U360" s="5"/>
     </row>
-    <row r="361" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A361" s="12">
         <v>359</v>
       </c>
@@ -14065,7 +14071,7 @@
       <c r="T361" s="3"/>
       <c r="U361" s="5"/>
     </row>
-    <row r="362" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A362" s="12">
         <v>360</v>
       </c>
@@ -14097,7 +14103,7 @@
       <c r="T362" s="3"/>
       <c r="U362" s="5"/>
     </row>
-    <row r="363" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A363" s="12">
         <v>361</v>
       </c>
@@ -14129,7 +14135,7 @@
       <c r="T363" s="3"/>
       <c r="U363" s="5"/>
     </row>
-    <row r="364" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A364" s="12">
         <v>362</v>
       </c>
@@ -14161,7 +14167,7 @@
       <c r="T364" s="3"/>
       <c r="U364" s="5"/>
     </row>
-    <row r="365" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A365" s="12">
         <v>363</v>
       </c>
@@ -14193,7 +14199,7 @@
       <c r="T365" s="3"/>
       <c r="U365" s="5"/>
     </row>
-    <row r="366" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A366" s="12">
         <v>364</v>
       </c>
@@ -14225,7 +14231,7 @@
       <c r="T366" s="3"/>
       <c r="U366" s="5"/>
     </row>
-    <row r="367" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A367" s="12">
         <v>365</v>
       </c>
@@ -14257,7 +14263,7 @@
       <c r="T367" s="3"/>
       <c r="U367" s="5"/>
     </row>
-    <row r="368" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A368" s="12">
         <v>366</v>
       </c>
@@ -14289,7 +14295,7 @@
       <c r="T368" s="3"/>
       <c r="U368" s="5"/>
     </row>
-    <row r="369" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A369" s="12">
         <v>367</v>
       </c>
@@ -14321,7 +14327,7 @@
       <c r="T369" s="3"/>
       <c r="U369" s="5"/>
     </row>
-    <row r="370" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A370" s="12">
         <v>368</v>
       </c>
@@ -14353,7 +14359,7 @@
       <c r="T370" s="3"/>
       <c r="U370" s="5"/>
     </row>
-    <row r="371" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A371" s="12">
         <v>369</v>
       </c>
@@ -14385,7 +14391,7 @@
       <c r="T371" s="3"/>
       <c r="U371" s="5"/>
     </row>
-    <row r="372" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A372" s="12">
         <v>370</v>
       </c>
@@ -14417,7 +14423,7 @@
       <c r="T372" s="3"/>
       <c r="U372" s="5"/>
     </row>
-    <row r="373" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A373" s="12">
         <v>371</v>
       </c>
@@ -14449,7 +14455,7 @@
       <c r="T373" s="3"/>
       <c r="U373" s="5"/>
     </row>
-    <row r="374" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A374" s="12">
         <v>372</v>
       </c>
@@ -14481,7 +14487,7 @@
       <c r="T374" s="3"/>
       <c r="U374" s="5"/>
     </row>
-    <row r="375" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A375" s="12">
         <v>373</v>
       </c>
@@ -14513,7 +14519,7 @@
       <c r="T375" s="3"/>
       <c r="U375" s="5"/>
     </row>
-    <row r="376" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A376" s="12">
         <v>374</v>
       </c>
@@ -14545,7 +14551,7 @@
       <c r="T376" s="3"/>
       <c r="U376" s="5"/>
     </row>
-    <row r="377" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A377" s="12">
         <v>375</v>
       </c>
@@ -14577,7 +14583,7 @@
       <c r="T377" s="3"/>
       <c r="U377" s="5"/>
     </row>
-    <row r="378" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A378" s="12">
         <v>376</v>
       </c>
@@ -14609,7 +14615,7 @@
       <c r="T378" s="3"/>
       <c r="U378" s="5"/>
     </row>
-    <row r="379" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A379" s="12">
         <v>377</v>
       </c>
@@ -14641,7 +14647,7 @@
       <c r="T379" s="3"/>
       <c r="U379" s="5"/>
     </row>
-    <row r="380" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="12">
         <v>378</v>
       </c>
@@ -14673,7 +14679,7 @@
       <c r="T380" s="3"/>
       <c r="U380" s="5"/>
     </row>
-    <row r="381" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A381" s="12">
         <v>379</v>
       </c>
@@ -14707,7 +14713,7 @@
       <c r="T381" s="3"/>
       <c r="U381" s="5"/>
     </row>
-    <row r="382" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A382" s="12">
         <v>380</v>
       </c>
@@ -14739,7 +14745,7 @@
       <c r="T382" s="3"/>
       <c r="U382" s="5"/>
     </row>
-    <row r="383" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A383" s="12">
         <v>381</v>
       </c>
@@ -14771,7 +14777,7 @@
       <c r="T383" s="3"/>
       <c r="U383" s="5"/>
     </row>
-    <row r="384" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A384" s="12">
         <v>382</v>
       </c>
@@ -14803,7 +14809,7 @@
       <c r="T384" s="3"/>
       <c r="U384" s="5"/>
     </row>
-    <row r="385" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A385" s="12">
         <v>383</v>
       </c>
@@ -14837,7 +14843,7 @@
       <c r="T385" s="3"/>
       <c r="U385" s="5"/>
     </row>
-    <row r="386" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A386" s="12">
         <v>384</v>
       </c>
@@ -14869,7 +14875,7 @@
       <c r="T386" s="3"/>
       <c r="U386" s="5"/>
     </row>
-    <row r="387" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A387" s="12">
         <v>385</v>
       </c>
@@ -14901,7 +14907,7 @@
       <c r="T387" s="3"/>
       <c r="U387" s="5"/>
     </row>
-    <row r="388" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A388" s="12">
         <v>386</v>
       </c>
@@ -14935,7 +14941,7 @@
       <c r="T388" s="3"/>
       <c r="U388" s="5"/>
     </row>
-    <row r="389" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A389" s="12">
         <v>387</v>
       </c>
@@ -14967,7 +14973,7 @@
       <c r="T389" s="3"/>
       <c r="U389" s="5"/>
     </row>
-    <row r="390" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A390" s="12">
         <v>388</v>
       </c>
@@ -14999,7 +15005,7 @@
       <c r="T390" s="3"/>
       <c r="U390" s="5"/>
     </row>
-    <row r="391" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A391" s="12">
         <v>389</v>
       </c>
@@ -15031,7 +15037,7 @@
       <c r="T391" s="3"/>
       <c r="U391" s="5"/>
     </row>
-    <row r="392" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A392" s="12">
         <v>390</v>
       </c>
@@ -15063,7 +15069,7 @@
       <c r="T392" s="3"/>
       <c r="U392" s="5"/>
     </row>
-    <row r="393" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A393" s="12">
         <v>391</v>
       </c>
@@ -15095,7 +15101,7 @@
       <c r="T393" s="3"/>
       <c r="U393" s="5"/>
     </row>
-    <row r="394" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A394" s="12">
         <v>392</v>
       </c>
@@ -15127,7 +15133,7 @@
       <c r="T394" s="3"/>
       <c r="U394" s="5"/>
     </row>
-    <row r="395" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A395" s="12">
         <v>393</v>
       </c>
@@ -15159,7 +15165,7 @@
       <c r="T395" s="3"/>
       <c r="U395" s="5"/>
     </row>
-    <row r="396" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A396" s="12">
         <v>394</v>
       </c>
@@ -15191,7 +15197,7 @@
       <c r="T396" s="3"/>
       <c r="U396" s="5"/>
     </row>
-    <row r="397" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A397" s="12">
         <v>395</v>
       </c>
@@ -15225,7 +15231,7 @@
       <c r="T397" s="3"/>
       <c r="U397" s="5"/>
     </row>
-    <row r="398" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A398" s="12">
         <v>396</v>
       </c>
@@ -15257,7 +15263,7 @@
       <c r="T398" s="3"/>
       <c r="U398" s="5"/>
     </row>
-    <row r="399" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A399" s="12">
         <v>397</v>
       </c>
@@ -15289,7 +15295,7 @@
       <c r="T399" s="3"/>
       <c r="U399" s="5"/>
     </row>
-    <row r="400" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A400" s="12">
         <v>398</v>
       </c>
@@ -15321,7 +15327,7 @@
       <c r="T400" s="3"/>
       <c r="U400" s="5"/>
     </row>
-    <row r="401" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A401" s="12">
         <v>399</v>
       </c>
@@ -15347,7 +15353,9 @@
       <c r="L401" s="3"/>
       <c r="M401" s="3"/>
       <c r="N401" s="3"/>
-      <c r="O401" s="3"/>
+      <c r="O401" s="3" t="s">
+        <v>548</v>
+      </c>
       <c r="P401" s="3"/>
       <c r="Q401" s="3"/>
       <c r="R401" s="3"/>
@@ -15355,7 +15363,7 @@
       <c r="T401" s="3"/>
       <c r="U401" s="5"/>
     </row>
-    <row r="402" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A402" s="12">
         <v>400</v>
       </c>
@@ -15389,7 +15397,7 @@
       <c r="T402" s="3"/>
       <c r="U402" s="5"/>
     </row>
-    <row r="403" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A403" s="12">
         <v>401</v>
       </c>
@@ -15421,7 +15429,7 @@
       <c r="T403" s="3"/>
       <c r="U403" s="5"/>
     </row>
-    <row r="404" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A404" s="12">
         <v>402</v>
       </c>
@@ -15455,7 +15463,7 @@
       <c r="T404" s="3"/>
       <c r="U404" s="5"/>
     </row>
-    <row r="405" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A405" s="12">
         <v>403</v>
       </c>
@@ -15487,7 +15495,7 @@
       <c r="T405" s="3"/>
       <c r="U405" s="5"/>
     </row>
-    <row r="406" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A406" s="12">
         <v>404</v>
       </c>
@@ -15519,7 +15527,7 @@
       <c r="T406" s="3"/>
       <c r="U406" s="5"/>
     </row>
-    <row r="407" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A407" s="12">
         <v>405</v>
       </c>
@@ -15551,7 +15559,7 @@
       <c r="T407" s="3"/>
       <c r="U407" s="5"/>
     </row>
-    <row r="408" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A408" s="12">
         <v>406</v>
       </c>
@@ -15583,7 +15591,7 @@
       <c r="T408" s="3"/>
       <c r="U408" s="5"/>
     </row>
-    <row r="409" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A409" s="12">
         <v>407</v>
       </c>
@@ -15615,7 +15623,7 @@
       <c r="T409" s="3"/>
       <c r="U409" s="5"/>
     </row>
-    <row r="410" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A410" s="12">
         <v>408</v>
       </c>
@@ -15649,7 +15657,7 @@
       <c r="T410" s="3"/>
       <c r="U410" s="5"/>
     </row>
-    <row r="411" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A411" s="12">
         <v>409</v>
       </c>
@@ -15683,7 +15691,7 @@
       <c r="T411" s="3"/>
       <c r="U411" s="5"/>
     </row>
-    <row r="412" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A412" s="12">
         <v>410</v>
       </c>
@@ -15717,7 +15725,7 @@
       <c r="T412" s="3"/>
       <c r="U412" s="5"/>
     </row>
-    <row r="413" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A413" s="12">
         <v>411</v>
       </c>
@@ -15751,7 +15759,7 @@
       <c r="T413" s="3"/>
       <c r="U413" s="5"/>
     </row>
-    <row r="414" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A414" s="12">
         <v>412</v>
       </c>
@@ -15785,7 +15793,7 @@
       <c r="T414" s="3"/>
       <c r="U414" s="5"/>
     </row>
-    <row r="415" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A415" s="12">
         <v>413</v>
       </c>
@@ -15821,7 +15829,7 @@
       <c r="T415" s="3"/>
       <c r="U415" s="5"/>
     </row>
-    <row r="416" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A416" s="12">
         <v>414</v>
       </c>
@@ -15853,7 +15861,7 @@
       <c r="T416" s="3"/>
       <c r="U416" s="5"/>
     </row>
-    <row r="417" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A417" s="12">
         <v>415</v>
       </c>
@@ -15885,7 +15893,7 @@
       <c r="T417" s="3"/>
       <c r="U417" s="5"/>
     </row>
-    <row r="418" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A418" s="12">
         <v>416</v>
       </c>
@@ -15923,7 +15931,7 @@
       <c r="T418" s="3"/>
       <c r="U418" s="5"/>
     </row>
-    <row r="419" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A419" s="12">
         <v>417</v>
       </c>
@@ -15961,7 +15969,7 @@
       <c r="T419" s="3"/>
       <c r="U419" s="5"/>
     </row>
-    <row r="420" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A420" s="12">
         <v>418</v>
       </c>
@@ -15999,7 +16007,7 @@
       <c r="T420" s="3"/>
       <c r="U420" s="5"/>
     </row>
-    <row r="421" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A421" s="12">
         <v>419</v>
       </c>
@@ -16037,7 +16045,7 @@
       <c r="T421" s="3"/>
       <c r="U421" s="5"/>
     </row>
-    <row r="422" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A422" s="12">
         <v>420</v>
       </c>
@@ -16075,7 +16083,7 @@
       <c r="T422" s="3"/>
       <c r="U422" s="5"/>
     </row>
-    <row r="423" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A423" s="12">
         <v>421</v>
       </c>
@@ -16113,7 +16121,7 @@
       <c r="T423" s="3"/>
       <c r="U423" s="5"/>
     </row>
-    <row r="424" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A424" s="12">
         <v>422</v>
       </c>
@@ -16153,7 +16161,7 @@
       <c r="T424" s="3"/>
       <c r="U424" s="5"/>
     </row>
-    <row r="425" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A425" s="12">
         <v>423</v>
       </c>
@@ -16191,7 +16199,7 @@
       <c r="T425" s="3"/>
       <c r="U425" s="5"/>
     </row>
-    <row r="426" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A426" s="12">
         <v>424</v>
       </c>
@@ -16231,7 +16239,7 @@
       <c r="T426" s="3"/>
       <c r="U426" s="5"/>
     </row>
-    <row r="427" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A427" s="12">
         <v>425</v>
       </c>
@@ -16269,7 +16277,7 @@
       <c r="T427" s="3"/>
       <c r="U427" s="5"/>
     </row>
-    <row r="428" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A428" s="12">
         <v>426</v>
       </c>
@@ -16307,7 +16315,7 @@
       <c r="T428" s="3"/>
       <c r="U428" s="5"/>
     </row>
-    <row r="429" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="12">
         <v>427</v>
       </c>
@@ -16347,7 +16355,7 @@
       <c r="T429" s="3"/>
       <c r="U429" s="5"/>
     </row>
-    <row r="430" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A430" s="12">
         <v>428</v>
       </c>
@@ -16387,7 +16395,7 @@
       <c r="T430" s="3"/>
       <c r="U430" s="5"/>
     </row>
-    <row r="431" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A431" s="12">
         <v>429</v>
       </c>
@@ -16425,7 +16433,7 @@
       <c r="T431" s="3"/>
       <c r="U431" s="5"/>
     </row>
-    <row r="432" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A432" s="12">
         <v>430</v>
       </c>
@@ -16465,7 +16473,7 @@
       <c r="T432" s="3"/>
       <c r="U432" s="5"/>
     </row>
-    <row r="433" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A433" s="12">
         <v>431</v>
       </c>
@@ -16503,7 +16511,7 @@
       <c r="T433" s="3"/>
       <c r="U433" s="5"/>
     </row>
-    <row r="434" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A434" s="12">
         <v>432</v>
       </c>
@@ -16543,7 +16551,7 @@
       <c r="T434" s="3"/>
       <c r="U434" s="5"/>
     </row>
-    <row r="435" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A435" s="12">
         <v>433</v>
       </c>
@@ -16583,7 +16591,7 @@
       <c r="T435" s="3"/>
       <c r="U435" s="5"/>
     </row>
-    <row r="436" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A436" s="12">
         <v>434</v>
       </c>
@@ -16619,7 +16627,7 @@
       <c r="T436" s="3"/>
       <c r="U436" s="5"/>
     </row>
-    <row r="437" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A437" s="12">
         <v>435</v>
       </c>
@@ -16655,7 +16663,7 @@
       <c r="T437" s="3"/>
       <c r="U437" s="5"/>
     </row>
-    <row r="438" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A438" s="12">
         <v>436</v>
       </c>
@@ -16691,7 +16699,7 @@
       <c r="T438" s="3"/>
       <c r="U438" s="5"/>
     </row>
-    <row r="439" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A439" s="12">
         <v>437</v>
       </c>
@@ -16727,7 +16735,7 @@
       <c r="T439" s="3"/>
       <c r="U439" s="5"/>
     </row>
-    <row r="440" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A440" s="12">
         <v>438</v>
       </c>
@@ -16763,7 +16771,7 @@
       <c r="T440" s="3"/>
       <c r="U440" s="5"/>
     </row>
-    <row r="441" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A441" s="12">
         <v>439</v>
       </c>
@@ -16799,7 +16807,7 @@
       <c r="T441" s="3"/>
       <c r="U441" s="5"/>
     </row>
-    <row r="442" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A442" s="12">
         <v>440</v>
       </c>
@@ -16833,7 +16841,7 @@
       <c r="T442" s="3"/>
       <c r="U442" s="5"/>
     </row>
-    <row r="443" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A443" s="12">
         <v>441</v>
       </c>
@@ -16867,7 +16875,7 @@
       <c r="T443" s="3"/>
       <c r="U443" s="5"/>
     </row>
-    <row r="444" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A444" s="12">
         <v>442</v>
       </c>
@@ -16903,7 +16911,7 @@
       <c r="T444" s="3"/>
       <c r="U444" s="5"/>
     </row>
-    <row r="445" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A445" s="12">
         <v>443</v>
       </c>
@@ -16935,7 +16943,7 @@
       <c r="T445" s="3"/>
       <c r="U445" s="5"/>
     </row>
-    <row r="446" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A446" s="12">
         <v>444</v>
       </c>
@@ -16969,7 +16977,7 @@
       <c r="T446" s="3"/>
       <c r="U446" s="5"/>
     </row>
-    <row r="447" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A447" s="12">
         <v>445</v>
       </c>
@@ -17005,7 +17013,7 @@
       <c r="T447" s="3"/>
       <c r="U447" s="5"/>
     </row>
-    <row r="448" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A448" s="12">
         <v>446</v>
       </c>
@@ -17041,7 +17049,7 @@
       <c r="T448" s="3"/>
       <c r="U448" s="5"/>
     </row>
-    <row r="449" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A449" s="12">
         <v>447</v>
       </c>
@@ -17075,7 +17083,7 @@
       <c r="T449" s="3"/>
       <c r="U449" s="5"/>
     </row>
-    <row r="450" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A450" s="12">
         <v>448</v>
       </c>
@@ -17111,7 +17119,7 @@
       <c r="T450" s="3"/>
       <c r="U450" s="5"/>
     </row>
-    <row r="451" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A451" s="12">
         <v>449</v>
       </c>
@@ -17147,7 +17155,7 @@
       <c r="T451" s="3"/>
       <c r="U451" s="5"/>
     </row>
-    <row r="452" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A452" s="12">
         <v>450</v>
       </c>
@@ -17181,7 +17189,7 @@
       <c r="T452" s="3"/>
       <c r="U452" s="5"/>
     </row>
-    <row r="453" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A453" s="12">
         <v>451</v>
       </c>
@@ -17215,7 +17223,7 @@
       <c r="T453" s="3"/>
       <c r="U453" s="5"/>
     </row>
-    <row r="454" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A454" s="12">
         <v>452</v>
       </c>
@@ -17251,7 +17259,7 @@
       <c r="T454" s="3"/>
       <c r="U454" s="5"/>
     </row>
-    <row r="455" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A455" s="12">
         <v>453</v>
       </c>
@@ -17285,7 +17293,7 @@
       <c r="T455" s="3"/>
       <c r="U455" s="5"/>
     </row>
-    <row r="456" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A456" s="12">
         <v>454</v>
       </c>
@@ -17325,7 +17333,7 @@
       <c r="T456" s="3"/>
       <c r="U456" s="5"/>
     </row>
-    <row r="457" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A457" s="12">
         <v>455</v>
       </c>
@@ -17406,7 +17414,7 @@
       <c r="T458" s="3"/>
       <c r="U458" s="5"/>
     </row>
-    <row r="459" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A459" s="12">
         <v>457</v>
       </c>
@@ -17442,7 +17450,7 @@
       <c r="T459" s="3"/>
       <c r="U459" s="5"/>
     </row>
-    <row r="460" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A460" s="12">
         <v>458</v>
       </c>
@@ -17482,7 +17490,7 @@
       <c r="T460" s="3"/>
       <c r="U460" s="5"/>
     </row>
-    <row r="461" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A461" s="12">
         <v>459</v>
       </c>
@@ -17522,7 +17530,7 @@
       <c r="T461" s="3"/>
       <c r="U461" s="5"/>
     </row>
-    <row r="462" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A462" s="12">
         <v>460</v>
       </c>
@@ -17558,7 +17566,7 @@
       <c r="T462" s="3"/>
       <c r="U462" s="5"/>
     </row>
-    <row r="463" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A463" s="12">
         <v>461</v>
       </c>
@@ -17594,7 +17602,7 @@
       <c r="T463" s="3"/>
       <c r="U463" s="5"/>
     </row>
-    <row r="464" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A464" s="12">
         <v>462</v>
       </c>
@@ -17630,7 +17638,7 @@
       <c r="T464" s="3"/>
       <c r="U464" s="5"/>
     </row>
-    <row r="465" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A465" s="12">
         <v>463</v>
       </c>
@@ -17666,7 +17674,7 @@
       <c r="T465" s="3"/>
       <c r="U465" s="5"/>
     </row>
-    <row r="466" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A466" s="12">
         <v>464</v>
       </c>
@@ -18665,7 +18673,7 @@
       <c r="T495" s="3"/>
       <c r="U495" s="5"/>
     </row>
-    <row r="496" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A496" s="12">
         <v>494</v>
       </c>
@@ -18699,7 +18707,7 @@
       <c r="T496" s="3"/>
       <c r="U496" s="5"/>
     </row>
-    <row r="497" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A497" s="12">
         <v>495</v>
       </c>
@@ -18733,7 +18741,7 @@
       <c r="T497" s="3"/>
       <c r="U497" s="5"/>
     </row>
-    <row r="498" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A498" s="12">
         <v>496</v>
       </c>
@@ -18769,7 +18777,7 @@
       <c r="T498" s="3"/>
       <c r="U498" s="5"/>
     </row>
-    <row r="499" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A499" s="12">
         <v>497</v>
       </c>
@@ -18805,7 +18813,7 @@
       <c r="T499" s="3"/>
       <c r="U499" s="5"/>
     </row>
-    <row r="500" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A500" s="12">
         <v>498</v>
       </c>
@@ -18839,7 +18847,7 @@
       <c r="T500" s="3"/>
       <c r="U500" s="5"/>
     </row>
-    <row r="501" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A501" s="12">
         <v>499</v>
       </c>
@@ -18871,7 +18879,7 @@
       <c r="T501" s="3"/>
       <c r="U501" s="5"/>
     </row>
-    <row r="502" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A502" s="12">
         <v>500</v>
       </c>
@@ -18903,7 +18911,7 @@
       <c r="T502" s="3"/>
       <c r="U502" s="5"/>
     </row>
-    <row r="503" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A503" s="12">
         <v>501</v>
       </c>
@@ -18935,7 +18943,7 @@
       <c r="T503" s="3"/>
       <c r="U503" s="5"/>
     </row>
-    <row r="504" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A504" s="12">
         <v>502</v>
       </c>
@@ -18967,7 +18975,7 @@
       <c r="T504" s="3"/>
       <c r="U504" s="5"/>
     </row>
-    <row r="505" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A505" s="12">
         <v>503</v>
       </c>
@@ -18999,7 +19007,7 @@
       <c r="T505" s="3"/>
       <c r="U505" s="5"/>
     </row>
-    <row r="506" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A506" s="12">
         <v>504</v>
       </c>
@@ -19031,7 +19039,7 @@
       <c r="T506" s="3"/>
       <c r="U506" s="5"/>
     </row>
-    <row r="507" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A507" s="12">
         <v>505</v>
       </c>
@@ -19063,7 +19071,7 @@
       <c r="T507" s="3"/>
       <c r="U507" s="5"/>
     </row>
-    <row r="508" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A508" s="12">
         <v>506</v>
       </c>
@@ -19095,7 +19103,7 @@
       <c r="T508" s="3"/>
       <c r="U508" s="5"/>
     </row>
-    <row r="509" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A509" s="12">
         <v>507</v>
       </c>
@@ -19127,7 +19135,7 @@
       <c r="T509" s="3"/>
       <c r="U509" s="5"/>
     </row>
-    <row r="510" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A510" s="12">
         <v>508</v>
       </c>
@@ -19159,7 +19167,7 @@
       <c r="T510" s="3"/>
       <c r="U510" s="5"/>
     </row>
-    <row r="511" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A511" s="12">
         <v>509</v>
       </c>
@@ -19191,7 +19199,7 @@
       <c r="T511" s="3"/>
       <c r="U511" s="5"/>
     </row>
-    <row r="512" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A512" s="12">
         <v>510</v>
       </c>
@@ -19223,7 +19231,7 @@
       <c r="T512" s="3"/>
       <c r="U512" s="5"/>
     </row>
-    <row r="513" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A513" s="12">
         <v>511</v>
       </c>
@@ -19255,7 +19263,7 @@
       <c r="T513" s="3"/>
       <c r="U513" s="5"/>
     </row>
-    <row r="514" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A514" s="12">
         <v>512</v>
       </c>
@@ -19287,7 +19295,7 @@
       <c r="T514" s="3"/>
       <c r="U514" s="5"/>
     </row>
-    <row r="515" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A515" s="12">
         <v>513</v>
       </c>
@@ -19319,7 +19327,7 @@
       <c r="T515" s="3"/>
       <c r="U515" s="5"/>
     </row>
-    <row r="516" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A516" s="12">
         <v>514</v>
       </c>
@@ -19351,7 +19359,7 @@
       <c r="T516" s="3"/>
       <c r="U516" s="5"/>
     </row>
-    <row r="517" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A517" s="12">
         <v>515</v>
       </c>
@@ -19383,7 +19391,7 @@
       <c r="T517" s="3"/>
       <c r="U517" s="5"/>
     </row>
-    <row r="518" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A518" s="12">
         <v>516</v>
       </c>
@@ -19415,7 +19423,7 @@
       <c r="T518" s="3"/>
       <c r="U518" s="5"/>
     </row>
-    <row r="519" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A519" s="12">
         <v>517</v>
       </c>
@@ -19447,7 +19455,7 @@
       <c r="T519" s="3"/>
       <c r="U519" s="5"/>
     </row>
-    <row r="520" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A520" s="12">
         <v>518</v>
       </c>
@@ -19479,7 +19487,7 @@
       <c r="T520" s="3"/>
       <c r="U520" s="5"/>
     </row>
-    <row r="521" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A521" s="12">
         <v>519</v>
       </c>
@@ -19511,7 +19519,7 @@
       <c r="T521" s="3"/>
       <c r="U521" s="5"/>
     </row>
-    <row r="522" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A522" s="12">
         <v>520</v>
       </c>
@@ -19543,7 +19551,7 @@
       <c r="T522" s="3"/>
       <c r="U522" s="5"/>
     </row>
-    <row r="523" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A523" s="12">
         <v>521</v>
       </c>
@@ -19575,7 +19583,7 @@
       <c r="T523" s="3"/>
       <c r="U523" s="5"/>
     </row>
-    <row r="524" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A524" s="12">
         <v>522</v>
       </c>
@@ -19607,7 +19615,7 @@
       <c r="T524" s="3"/>
       <c r="U524" s="5"/>
     </row>
-    <row r="525" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A525" s="12">
         <v>523</v>
       </c>
@@ -19639,7 +19647,7 @@
       <c r="T525" s="3"/>
       <c r="U525" s="5"/>
     </row>
-    <row r="526" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A526" s="12">
         <v>524</v>
       </c>
@@ -19671,7 +19679,7 @@
       <c r="T526" s="3"/>
       <c r="U526" s="5"/>
     </row>
-    <row r="527" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A527" s="12">
         <v>525</v>
       </c>
@@ -19703,7 +19711,7 @@
       <c r="T527" s="3"/>
       <c r="U527" s="5"/>
     </row>
-    <row r="528" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A528" s="12">
         <v>526</v>
       </c>
@@ -19735,7 +19743,7 @@
       <c r="T528" s="3"/>
       <c r="U528" s="5"/>
     </row>
-    <row r="529" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A529" s="12">
         <v>527</v>
       </c>
@@ -19767,7 +19775,7 @@
       <c r="T529" s="3"/>
       <c r="U529" s="5"/>
     </row>
-    <row r="530" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A530" s="12">
         <v>528</v>
       </c>
@@ -19799,7 +19807,7 @@
       <c r="T530" s="3"/>
       <c r="U530" s="5"/>
     </row>
-    <row r="531" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A531" s="12">
         <v>529</v>
       </c>
@@ -19831,7 +19839,7 @@
       <c r="T531" s="3"/>
       <c r="U531" s="5"/>
     </row>
-    <row r="532" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A532" s="12">
         <v>530</v>
       </c>
@@ -19863,7 +19871,7 @@
       <c r="T532" s="3"/>
       <c r="U532" s="5"/>
     </row>
-    <row r="533" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A533" s="12">
         <v>531</v>
       </c>
@@ -19895,7 +19903,7 @@
       <c r="T533" s="3"/>
       <c r="U533" s="5"/>
     </row>
-    <row r="534" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A534" s="12">
         <v>532</v>
       </c>
@@ -19927,7 +19935,7 @@
       <c r="T534" s="3"/>
       <c r="U534" s="5"/>
     </row>
-    <row r="535" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A535" s="12">
         <v>533</v>
       </c>
@@ -19959,7 +19967,7 @@
       <c r="T535" s="3"/>
       <c r="U535" s="5"/>
     </row>
-    <row r="536" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A536" s="12">
         <v>534</v>
       </c>
@@ -19991,7 +19999,7 @@
       <c r="T536" s="3"/>
       <c r="U536" s="5"/>
     </row>
-    <row r="537" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A537" s="12">
         <v>535</v>
       </c>
@@ -20023,7 +20031,7 @@
       <c r="T537" s="3"/>
       <c r="U537" s="5"/>
     </row>
-    <row r="538" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A538" s="12">
         <v>536</v>
       </c>
@@ -20055,7 +20063,7 @@
       <c r="T538" s="3"/>
       <c r="U538" s="5"/>
     </row>
-    <row r="539" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A539" s="12">
         <v>537</v>
       </c>
@@ -20087,7 +20095,7 @@
       <c r="T539" s="3"/>
       <c r="U539" s="5"/>
     </row>
-    <row r="540" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A540" s="12">
         <v>538</v>
       </c>
@@ -20119,7 +20127,7 @@
       <c r="T540" s="3"/>
       <c r="U540" s="5"/>
     </row>
-    <row r="541" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A541" s="12">
         <v>539</v>
       </c>
@@ -20151,7 +20159,7 @@
       <c r="T541" s="3"/>
       <c r="U541" s="5"/>
     </row>
-    <row r="542" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A542" s="12">
         <v>540</v>
       </c>
@@ -20183,7 +20191,7 @@
       <c r="T542" s="3"/>
       <c r="U542" s="5"/>
     </row>
-    <row r="543" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A543" s="12">
         <v>541</v>
       </c>
@@ -20215,7 +20223,7 @@
       <c r="T543" s="3"/>
       <c r="U543" s="5"/>
     </row>
-    <row r="544" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A544" s="12">
         <v>542</v>
       </c>
@@ -20247,7 +20255,7 @@
       <c r="T544" s="3"/>
       <c r="U544" s="5"/>
     </row>
-    <row r="545" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A545" s="12">
         <v>543</v>
       </c>
@@ -20279,7 +20287,7 @@
       <c r="T545" s="3"/>
       <c r="U545" s="5"/>
     </row>
-    <row r="546" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A546" s="12">
         <v>544</v>
       </c>
@@ -20311,7 +20319,7 @@
       <c r="T546" s="3"/>
       <c r="U546" s="5"/>
     </row>
-    <row r="547" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A547" s="12">
         <v>545</v>
       </c>
@@ -20343,7 +20351,7 @@
       <c r="T547" s="3"/>
       <c r="U547" s="5"/>
     </row>
-    <row r="548" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A548" s="12">
         <v>546</v>
       </c>
@@ -20375,7 +20383,7 @@
       <c r="T548" s="3"/>
       <c r="U548" s="5"/>
     </row>
-    <row r="549" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A549" s="12">
         <v>547</v>
       </c>
@@ -20407,7 +20415,7 @@
       <c r="T549" s="3"/>
       <c r="U549" s="5"/>
     </row>
-    <row r="550" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A550" s="12">
         <v>548</v>
       </c>
@@ -20439,7 +20447,7 @@
       <c r="T550" s="3"/>
       <c r="U550" s="5"/>
     </row>
-    <row r="551" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A551" s="12">
         <v>549</v>
       </c>
@@ -20471,7 +20479,7 @@
       <c r="T551" s="3"/>
       <c r="U551" s="5"/>
     </row>
-    <row r="552" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A552" s="12">
         <v>550</v>
       </c>
@@ -20503,7 +20511,7 @@
       <c r="T552" s="3"/>
       <c r="U552" s="5"/>
     </row>
-    <row r="553" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A553" s="12">
         <v>551</v>
       </c>
@@ -20535,7 +20543,7 @@
       <c r="T553" s="3"/>
       <c r="U553" s="5"/>
     </row>
-    <row r="554" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A554" s="12">
         <v>552</v>
       </c>
@@ -20567,7 +20575,7 @@
       <c r="T554" s="3"/>
       <c r="U554" s="5"/>
     </row>
-    <row r="555" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A555" s="12">
         <v>553</v>
       </c>
@@ -20599,7 +20607,7 @@
       <c r="T555" s="3"/>
       <c r="U555" s="5"/>
     </row>
-    <row r="556" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A556" s="12">
         <v>554</v>
       </c>
@@ -20631,7 +20639,7 @@
       <c r="T556" s="3"/>
       <c r="U556" s="5"/>
     </row>
-    <row r="557" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A557" s="12">
         <v>555</v>
       </c>
@@ -20663,7 +20671,7 @@
       <c r="T557" s="3"/>
       <c r="U557" s="5"/>
     </row>
-    <row r="558" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A558" s="12">
         <v>556</v>
       </c>
@@ -20695,7 +20703,7 @@
       <c r="T558" s="3"/>
       <c r="U558" s="5"/>
     </row>
-    <row r="559" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A559" s="12">
         <v>557</v>
       </c>
@@ -20727,7 +20735,7 @@
       <c r="T559" s="3"/>
       <c r="U559" s="5"/>
     </row>
-    <row r="560" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A560" s="12">
         <v>558</v>
       </c>
@@ -20759,7 +20767,7 @@
       <c r="T560" s="3"/>
       <c r="U560" s="5"/>
     </row>
-    <row r="561" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A561" s="13">
         <v>559</v>
       </c>
@@ -20791,7 +20799,7 @@
       <c r="T561" s="7"/>
       <c r="U561" s="8"/>
     </row>
-    <row r="562" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A562" s="12">
         <v>560</v>
       </c>
@@ -20812,7 +20820,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="563" spans="1:21" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A563" s="13">
         <v>561</v>
       </c>
@@ -20837,7 +20845,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="564" spans="1:21" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:21" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A564" s="12">
         <v>562</v>
       </c>
@@ -20862,7 +20870,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="565" spans="1:21" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A565" s="13">
         <v>563</v>
       </c>
@@ -20887,7 +20895,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="566" spans="1:21" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A566" s="12">
         <v>564</v>
       </c>
@@ -20915,7 +20923,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="567" spans="1:21" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A567" s="13">
         <v>565</v>
       </c>
@@ -20940,7 +20948,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="568" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A568" s="12">
         <v>566</v>
       </c>
@@ -20964,7 +20972,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="569" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A569" s="13">
         <v>567</v>
       </c>
@@ -20994,7 +21002,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="570" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A570" s="12">
         <v>568</v>
       </c>
@@ -21018,50 +21026,44 @@
         <v>539</v>
       </c>
     </row>
-    <row r="571" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A571" s="13">
         <v>569</v>
       </c>
       <c r="C571" s="3"/>
     </row>
-    <row r="572" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A572" s="12">
         <v>570</v>
       </c>
       <c r="C572" s="3"/>
     </row>
-    <row r="573" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A573" s="13">
         <v>571</v>
       </c>
       <c r="C573" s="3"/>
     </row>
-    <row r="574" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A574" s="12">
         <v>572</v>
       </c>
       <c r="C574" s="3"/>
     </row>
-    <row r="575" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A575" s="13">
         <v>573</v>
       </c>
       <c r="C575" s="3"/>
     </row>
-    <row r="576" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A576" s="12">
         <v>574</v>
       </c>
       <c r="C576" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U576" xr:uid="{976D048D-26A2-4D77-A964-2445B5CE5606}">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U576" xr:uid="{976D048D-26A2-4D77-A964-2445B5CE5606}"/>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>

</xml_diff>

<commit_message>
baseline update due to DSI changes. for case 50517- change in exception which are good
</commit_message>
<xml_diff>
--- a/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
+++ b/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\baseline\outputbaselines\1.TestCaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E966C9AB-6EB6-4640-999C-22A2A9A1A50C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252EAD8A-771F-4D5B-ADD9-EC79792B108B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="551">
   <si>
     <t>S.No.</t>
   </si>
@@ -1707,6 +1707,12 @@
   </si>
   <si>
     <t>updated Min/Multiple qty for item=5001</t>
+  </si>
+  <si>
+    <t>10-Nov[2]</t>
+  </si>
+  <si>
+    <t>Change in exception table; results are good.</t>
   </si>
 </sst>
 </file>
@@ -1922,7 +1928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1955,15 +1961,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1983,6 +1980,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1993,6 +1993,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2483,10 +2492,10 @@
   <dimension ref="A1:U576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C384" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C538" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F391" sqref="F391"/>
+      <selection pane="bottomRight" activeCell="Q570" sqref="Q570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2498,62 +2507,68 @@
     <col min="5" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28">
         <v>44426</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="28">
         <v>44440</v>
       </c>
-      <c r="F1" s="16">
+      <c r="F1" s="28">
         <v>44452</v>
       </c>
-      <c r="G1" s="16">
+      <c r="G1" s="28">
         <v>44453</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="28">
         <v>44456</v>
       </c>
-      <c r="I1" s="16">
+      <c r="I1" s="28">
         <v>44467</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="23" t="s">
         <v>538</v>
       </c>
-      <c r="K1" s="16">
+      <c r="K1" s="28">
         <v>44468</v>
       </c>
-      <c r="L1" s="16">
+      <c r="L1" s="28">
         <v>44469</v>
       </c>
-      <c r="M1" s="16">
+      <c r="M1" s="28">
         <v>44479</v>
       </c>
-      <c r="N1" s="16">
+      <c r="N1" s="28">
         <v>44508</v>
       </c>
-      <c r="O1" s="16">
+      <c r="O1" s="28">
         <v>44510</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="15"/>
+      <c r="P1" s="28" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q1" s="28">
+        <v>44511</v>
+      </c>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -5442,7 +5457,7 @@
         <v>539</v>
       </c>
       <c r="K92" s="3"/>
-      <c r="L92" s="24" t="s">
+      <c r="L92" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M92" s="3"/>
@@ -5476,7 +5491,7 @@
         <v>539</v>
       </c>
       <c r="K93" s="3"/>
-      <c r="L93" s="24" t="s">
+      <c r="L93" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M93" s="3"/>
@@ -5542,7 +5557,7 @@
         <v>539</v>
       </c>
       <c r="K95" s="3"/>
-      <c r="L95" s="24" t="s">
+      <c r="L95" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M95" s="3"/>
@@ -5576,7 +5591,7 @@
         <v>539</v>
       </c>
       <c r="K96" s="3"/>
-      <c r="L96" s="24" t="s">
+      <c r="L96" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M96" s="3"/>
@@ -6474,7 +6489,7 @@
         <v>493</v>
       </c>
       <c r="K124" s="3"/>
-      <c r="L124" s="24" t="s">
+      <c r="L124" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M124" s="3"/>
@@ -14700,7 +14715,7 @@
         <v>539</v>
       </c>
       <c r="K381" s="3"/>
-      <c r="L381" s="24" t="s">
+      <c r="L381" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M381" s="3"/>
@@ -14830,7 +14845,7 @@
         <v>539</v>
       </c>
       <c r="K385" s="3"/>
-      <c r="L385" s="24" t="s">
+      <c r="L385" s="21" t="s">
         <v>544</v>
       </c>
       <c r="M385" s="3"/>
@@ -14928,7 +14943,7 @@
         <v>539</v>
       </c>
       <c r="K388" s="3"/>
-      <c r="L388" s="24" t="s">
+      <c r="L388" s="21" t="s">
         <v>469</v>
       </c>
       <c r="M388" s="3"/>
@@ -15218,7 +15233,7 @@
         <v>539</v>
       </c>
       <c r="K397" s="3"/>
-      <c r="L397" s="24" t="s">
+      <c r="L397" s="21" t="s">
         <v>469</v>
       </c>
       <c r="M397" s="3"/>
@@ -15704,7 +15719,7 @@
       </c>
       <c r="D412" s="3"/>
       <c r="E412" s="3"/>
-      <c r="F412" s="19" t="s">
+      <c r="F412" s="16" t="s">
         <v>497</v>
       </c>
       <c r="G412" s="3"/>
@@ -15897,7 +15912,7 @@
       <c r="A418" s="12">
         <v>416</v>
       </c>
-      <c r="B418" s="21">
+      <c r="B418" s="18">
         <v>50119</v>
       </c>
       <c r="C418" s="3" t="str">
@@ -15906,7 +15921,7 @@
       </c>
       <c r="D418" s="3"/>
       <c r="E418" s="3"/>
-      <c r="F418" s="19" t="s">
+      <c r="F418" s="16" t="s">
         <v>501</v>
       </c>
       <c r="G418" s="3" t="s">
@@ -15951,7 +15966,7 @@
         <v>526</v>
       </c>
       <c r="H419" s="3"/>
-      <c r="I419" s="24" t="s">
+      <c r="I419" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J419" s="3" t="s">
@@ -15989,7 +16004,7 @@
         <v>526</v>
       </c>
       <c r="H420" s="3"/>
-      <c r="I420" s="24" t="s">
+      <c r="I420" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J420" s="3" t="s">
@@ -16027,7 +16042,7 @@
         <v>526</v>
       </c>
       <c r="H421" s="3"/>
-      <c r="I421" s="24" t="s">
+      <c r="I421" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J421" s="3" t="s">
@@ -16065,7 +16080,7 @@
         <v>526</v>
       </c>
       <c r="H422" s="3"/>
-      <c r="I422" s="24" t="s">
+      <c r="I422" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J422" s="3" t="s">
@@ -16096,14 +16111,14 @@
       </c>
       <c r="D423" s="3"/>
       <c r="E423" s="3"/>
-      <c r="F423" s="22" t="s">
+      <c r="F423" s="19" t="s">
         <v>503</v>
       </c>
       <c r="G423" s="3" t="s">
         <v>527</v>
       </c>
       <c r="H423" s="3"/>
-      <c r="I423" s="24" t="s">
+      <c r="I423" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J423" s="3" t="s">
@@ -16141,7 +16156,7 @@
         <v>515</v>
       </c>
       <c r="H424" s="3"/>
-      <c r="I424" s="24" t="s">
+      <c r="I424" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J424" s="3" t="s">
@@ -16174,14 +16189,14 @@
       </c>
       <c r="D425" s="3"/>
       <c r="E425" s="3"/>
-      <c r="F425" s="22" t="s">
+      <c r="F425" s="19" t="s">
         <v>504</v>
       </c>
       <c r="G425" s="3" t="s">
         <v>528</v>
       </c>
       <c r="H425" s="3"/>
-      <c r="I425" s="24" t="s">
+      <c r="I425" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J425" s="3" t="s">
@@ -16212,20 +16227,20 @@
       </c>
       <c r="D426" s="3"/>
       <c r="E426" s="3"/>
-      <c r="F426" s="22" t="s">
+      <c r="F426" s="19" t="s">
         <v>505</v>
       </c>
       <c r="G426" s="3" t="s">
         <v>529</v>
       </c>
       <c r="H426" s="3"/>
-      <c r="I426" s="24" t="s">
+      <c r="I426" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J426" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K426" s="25" t="s">
+      <c r="K426" s="22" t="s">
         <v>541</v>
       </c>
       <c r="L426" s="3"/>
@@ -16259,7 +16274,7 @@
       </c>
       <c r="G427" s="3"/>
       <c r="H427" s="3"/>
-      <c r="I427" s="24" t="s">
+      <c r="I427" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J427" s="3" t="s">
@@ -16297,7 +16312,7 @@
         <v>515</v>
       </c>
       <c r="H428" s="3"/>
-      <c r="I428" s="24" t="s">
+      <c r="I428" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J428" s="3" t="s">
@@ -16330,14 +16345,14 @@
         <v>460</v>
       </c>
       <c r="E429" s="3"/>
-      <c r="F429" s="19" t="s">
+      <c r="F429" s="16" t="s">
         <v>508</v>
       </c>
       <c r="G429" s="3" t="s">
         <v>519</v>
       </c>
       <c r="H429" s="3"/>
-      <c r="I429" s="24" t="s">
+      <c r="I429" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J429" s="3" t="s">
@@ -16370,14 +16385,14 @@
         <v>461</v>
       </c>
       <c r="E430" s="3"/>
-      <c r="F430" s="19" t="s">
+      <c r="F430" s="16" t="s">
         <v>509</v>
       </c>
       <c r="G430" s="3" t="s">
         <v>519</v>
       </c>
       <c r="H430" s="3"/>
-      <c r="I430" s="24" t="s">
+      <c r="I430" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J430" s="3" t="s">
@@ -16415,7 +16430,7 @@
         <v>530</v>
       </c>
       <c r="H431" s="3"/>
-      <c r="I431" s="24" t="s">
+      <c r="I431" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J431" s="3" t="s">
@@ -16448,14 +16463,14 @@
         <v>462</v>
       </c>
       <c r="E432" s="3"/>
-      <c r="F432" s="19" t="s">
+      <c r="F432" s="16" t="s">
         <v>511</v>
       </c>
       <c r="G432" s="3" t="s">
         <v>519</v>
       </c>
       <c r="H432" s="3"/>
-      <c r="I432" s="24" t="s">
+      <c r="I432" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J432" s="3" t="s">
@@ -16493,7 +16508,7 @@
         <v>530</v>
       </c>
       <c r="H433" s="3"/>
-      <c r="I433" s="24" t="s">
+      <c r="I433" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J433" s="3" t="s">
@@ -16526,14 +16541,14 @@
         <v>461</v>
       </c>
       <c r="E434" s="3"/>
-      <c r="F434" s="19" t="s">
+      <c r="F434" s="16" t="s">
         <v>512</v>
       </c>
       <c r="G434" s="3" t="s">
         <v>519</v>
       </c>
       <c r="H434" s="3"/>
-      <c r="I434" s="24" t="s">
+      <c r="I434" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J434" s="3" t="s">
@@ -16573,7 +16588,7 @@
         <v>531</v>
       </c>
       <c r="H435" s="3"/>
-      <c r="I435" s="24" t="s">
+      <c r="I435" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J435" s="3" t="s">
@@ -16886,7 +16901,7 @@
         <f>_xlfn.XLOOKUP(B444,[1]Sheet2!$A$2:$A$32,[1]Sheet2!$A$2:$A$32, "")</f>
         <v/>
       </c>
-      <c r="D444" s="20" t="s">
+      <c r="D444" s="17" t="s">
         <v>468</v>
       </c>
       <c r="E444" s="3"/>
@@ -17313,7 +17328,7 @@
         <v>530</v>
       </c>
       <c r="H456" s="3"/>
-      <c r="I456" s="24" t="s">
+      <c r="I456" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J456" s="3" t="s">
@@ -17355,13 +17370,13 @@
         <v>519</v>
       </c>
       <c r="H457" s="3"/>
-      <c r="I457" s="24" t="s">
+      <c r="I457" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J457" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="K457" s="25" t="s">
+      <c r="K457" s="22" t="s">
         <v>542</v>
       </c>
       <c r="L457" s="3"/>
@@ -17390,11 +17405,11 @@
       <c r="F458" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="G458" s="19" t="s">
+      <c r="G458" s="16" t="s">
         <v>532</v>
       </c>
       <c r="H458" s="3"/>
-      <c r="I458" s="24" t="s">
+      <c r="I458" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J458" s="3" t="s">
@@ -17429,7 +17444,7 @@
         <v>478</v>
       </c>
       <c r="E459" s="3"/>
-      <c r="F459" s="19" t="s">
+      <c r="F459" s="16" t="s">
         <v>520</v>
       </c>
       <c r="G459" s="3"/>
@@ -17470,7 +17485,7 @@
         <v>530</v>
       </c>
       <c r="H460" s="3"/>
-      <c r="I460" s="24" t="s">
+      <c r="I460" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J460" s="3" t="s">
@@ -17510,7 +17525,7 @@
         <v>530</v>
       </c>
       <c r="H461" s="3"/>
-      <c r="I461" s="24" t="s">
+      <c r="I461" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J461" s="3" t="s">
@@ -18558,7 +18573,7 @@
       <c r="J492" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="K492" s="24" t="s">
+      <c r="K492" s="21" t="s">
         <v>543</v>
       </c>
       <c r="L492" s="3"/>
@@ -18593,7 +18608,7 @@
       <c r="J493" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="K493" s="24" t="s">
+      <c r="K493" s="21" t="s">
         <v>543</v>
       </c>
       <c r="L493" s="3"/>
@@ -20831,14 +20846,14 @@
         <f>_xlfn.XLOOKUP(B563,[1]Sheet2!$A$2:$A$32,[1]Sheet2!$A$2:$A$32, "")</f>
         <v/>
       </c>
-      <c r="D563" s="17"/>
+      <c r="D563" s="14"/>
       <c r="E563" t="s">
         <v>488</v>
       </c>
       <c r="F563" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G563" s="23" t="s">
+      <c r="G563" s="20" t="s">
         <v>533</v>
       </c>
       <c r="J563" s="3" t="s">
@@ -20856,14 +20871,14 @@
         <f>_xlfn.XLOOKUP(B564,[1]Sheet2!$A$2:$A$32,[1]Sheet2!$A$2:$A$32, "")</f>
         <v/>
       </c>
-      <c r="D564" s="17"/>
+      <c r="D564" s="14"/>
       <c r="E564" t="s">
         <v>488</v>
       </c>
       <c r="F564" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G564" s="23" t="s">
+      <c r="G564" s="20" t="s">
         <v>533</v>
       </c>
       <c r="J564" s="3" t="s">
@@ -20874,21 +20889,21 @@
       <c r="A565" s="13">
         <v>563</v>
       </c>
-      <c r="B565" s="18" t="s">
+      <c r="B565" s="15" t="s">
         <v>482</v>
       </c>
       <c r="C565" s="3" t="str">
         <f>_xlfn.XLOOKUP(B565,[1]Sheet2!$A$2:$A$32,[1]Sheet2!$A$2:$A$32, "")</f>
         <v/>
       </c>
-      <c r="D565" s="17"/>
+      <c r="D565" s="14"/>
       <c r="E565" t="s">
         <v>489</v>
       </c>
       <c r="F565" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G565" s="23" t="s">
+      <c r="G565" s="20" t="s">
         <v>533</v>
       </c>
       <c r="J565" s="3" t="s">
@@ -20899,24 +20914,24 @@
       <c r="A566" s="12">
         <v>564</v>
       </c>
-      <c r="B566" s="18" t="s">
+      <c r="B566" s="15" t="s">
         <v>483</v>
       </c>
       <c r="C566" s="3" t="str">
         <f>_xlfn.XLOOKUP(B566,[1]Sheet2!$A$2:$A$32,[1]Sheet2!$A$2:$A$32, "")</f>
         <v/>
       </c>
-      <c r="D566" s="17"/>
+      <c r="D566" s="14"/>
       <c r="E566" t="s">
         <v>490</v>
       </c>
       <c r="F566" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="G566" s="23" t="s">
+      <c r="G566" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="I566" s="24" t="s">
+      <c r="I566" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J566" s="3" t="s">
@@ -20927,21 +20942,21 @@
       <c r="A567" s="13">
         <v>565</v>
       </c>
-      <c r="B567" s="18" t="s">
+      <c r="B567" s="15" t="s">
         <v>484</v>
       </c>
       <c r="C567" s="3" t="str">
         <f>_xlfn.XLOOKUP(B567,[1]Sheet2!$A$2:$A$32,[1]Sheet2!$A$2:$A$32, "")</f>
         <v/>
       </c>
-      <c r="D567" s="17"/>
+      <c r="D567" s="14"/>
       <c r="E567" t="s">
         <v>491</v>
       </c>
       <c r="F567" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G567" s="23" t="s">
+      <c r="G567" s="20" t="s">
         <v>533</v>
       </c>
       <c r="J567" s="3" t="s">
@@ -20965,7 +20980,7 @@
       <c r="F568" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G568" s="23" t="s">
+      <c r="G568" s="20" t="s">
         <v>533</v>
       </c>
       <c r="J568" s="3" t="s">
@@ -20976,7 +20991,7 @@
       <c r="A569" s="13">
         <v>567</v>
       </c>
-      <c r="B569" s="18" t="s">
+      <c r="B569" s="15" t="s">
         <v>486</v>
       </c>
       <c r="C569" s="3" t="str">
@@ -20989,10 +21004,10 @@
       <c r="F569" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G569" s="23" t="s">
+      <c r="G569" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="I569" s="24" t="s">
+      <c r="I569" s="21" t="s">
         <v>537</v>
       </c>
       <c r="J569" s="3" t="s">
@@ -21000,6 +21015,9 @@
       </c>
       <c r="L569" t="s">
         <v>546</v>
+      </c>
+      <c r="Q569" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="570" spans="1:21" x14ac:dyDescent="0.25">
@@ -21019,7 +21037,7 @@
       <c r="F570" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="G570" s="23" t="s">
+      <c r="G570" s="20" t="s">
         <v>533</v>
       </c>
       <c r="J570" s="3" t="s">

</xml_diff>

<commit_message>
changes in 6 cases due to desiredqty in roundingrules impacting load building. there are 8 cases in recalc and AVO-50501 which are also failing but not baselined https://github.com/JDA-Product-Development/plan-lrr-dcro/pull/213
</commit_message>
<xml_diff>
--- a/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
+++ b/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\baseline\outputbaselines\1.TestCaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252EAD8A-771F-4D5B-ADD9-EC79792B108B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB74BC-CDF6-4E2D-957A-E7533EE3836E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="552">
   <si>
     <t>S.No.</t>
   </si>
@@ -1713,6 +1713,9 @@
   </si>
   <si>
     <t>Change in exception table; results are good.</t>
+  </si>
+  <si>
+    <t>Changes due to shiproundingrules change for single source</t>
   </si>
 </sst>
 </file>
@@ -1983,6 +1986,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1993,15 +2005,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2492,10 +2495,10 @@
   <dimension ref="A1:U576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C538" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C440" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q570" sqref="Q570"/>
+      <selection pane="bottomRight" activeCell="A459" sqref="A459:XFD459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,66 +2512,69 @@
     <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24">
         <v>44426</v>
       </c>
-      <c r="E1" s="28">
+      <c r="E1" s="24">
         <v>44440</v>
       </c>
-      <c r="F1" s="28">
+      <c r="F1" s="24">
         <v>44452</v>
       </c>
-      <c r="G1" s="28">
+      <c r="G1" s="24">
         <v>44453</v>
       </c>
-      <c r="H1" s="28">
+      <c r="H1" s="24">
         <v>44456</v>
       </c>
-      <c r="I1" s="28">
+      <c r="I1" s="24">
         <v>44467</v>
       </c>
       <c r="J1" s="23" t="s">
         <v>538</v>
       </c>
-      <c r="K1" s="28">
+      <c r="K1" s="24">
         <v>44468</v>
       </c>
-      <c r="L1" s="28">
+      <c r="L1" s="24">
         <v>44469</v>
       </c>
-      <c r="M1" s="28">
+      <c r="M1" s="24">
         <v>44479</v>
       </c>
-      <c r="N1" s="28">
+      <c r="N1" s="24">
         <v>44508</v>
       </c>
-      <c r="O1" s="28">
+      <c r="O1" s="24">
         <v>44510</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="Q1" s="28">
+      <c r="Q1" s="24">
         <v>44511</v>
       </c>
-      <c r="R1" s="23"/>
+      <c r="R1" s="24">
+        <v>44533</v>
+      </c>
       <c r="S1" s="23"/>
       <c r="T1" s="23"/>
-      <c r="U1" s="29"/>
+      <c r="U1" s="25"/>
     </row>
     <row r="2" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -2680,7 +2686,9 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="R5" s="3" t="s">
+        <v>551</v>
+      </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="5"/>
@@ -16365,7 +16373,9 @@
       <c r="O429" s="3"/>
       <c r="P429" s="3"/>
       <c r="Q429" s="3"/>
-      <c r="R429" s="3"/>
+      <c r="R429" s="3" t="s">
+        <v>551</v>
+      </c>
       <c r="S429" s="3"/>
       <c r="T429" s="3"/>
       <c r="U429" s="5"/>
@@ -16601,7 +16611,9 @@
       <c r="O435" s="3"/>
       <c r="P435" s="3"/>
       <c r="Q435" s="3"/>
-      <c r="R435" s="3"/>
+      <c r="R435" s="3" t="s">
+        <v>551</v>
+      </c>
       <c r="S435" s="3"/>
       <c r="T435" s="3"/>
       <c r="U435" s="5"/>
@@ -17385,7 +17397,9 @@
       <c r="O457" s="3"/>
       <c r="P457" s="3"/>
       <c r="Q457" s="3"/>
-      <c r="R457" s="3"/>
+      <c r="R457" s="3" t="s">
+        <v>551</v>
+      </c>
       <c r="S457" s="3"/>
       <c r="T457" s="3"/>
       <c r="U457" s="5"/>
@@ -17424,7 +17438,9 @@
       <c r="O458" s="3"/>
       <c r="P458" s="3"/>
       <c r="Q458" s="3"/>
-      <c r="R458" s="3"/>
+      <c r="R458" s="3" t="s">
+        <v>551</v>
+      </c>
       <c r="S458" s="3"/>
       <c r="T458" s="3"/>
       <c r="U458" s="5"/>
@@ -17460,7 +17476,9 @@
       <c r="O459" s="3"/>
       <c r="P459" s="3"/>
       <c r="Q459" s="3"/>
-      <c r="R459" s="3"/>
+      <c r="R459" s="3" t="s">
+        <v>551</v>
+      </c>
       <c r="S459" s="3"/>
       <c r="T459" s="3"/>
       <c r="U459" s="5"/>

</xml_diff>

<commit_message>
new cases for multi-layer rounding cases from 50521-50532 50529- will be failing due to some issue. needs to be baselined
</commit_message>
<xml_diff>
--- a/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
+++ b/outputbaselines/1.TestCaseUpdate/All_BaselineUpdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\baseline\outputbaselines\1.TestCaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB74BC-CDF6-4E2D-957A-E7533EE3836E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B22161-A138-4F50-8393-9160977E9DE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{572F3A34-0A95-47C2-BCC7-F20876BFB9A5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="565">
   <si>
     <t>S.No.</t>
   </si>
@@ -1716,6 +1716,45 @@
   </si>
   <si>
     <t>Changes due to shiproundingrules change for single source</t>
+  </si>
+  <si>
+    <t>MLR-50521</t>
+  </si>
+  <si>
+    <t>MLR-50522</t>
+  </si>
+  <si>
+    <t>MLR-50523</t>
+  </si>
+  <si>
+    <t>MLR-50524</t>
+  </si>
+  <si>
+    <t>MLR-50525</t>
+  </si>
+  <si>
+    <t>MLR-50526</t>
+  </si>
+  <si>
+    <t>MLR-50527</t>
+  </si>
+  <si>
+    <t>MLR-50528</t>
+  </si>
+  <si>
+    <t>MLR-50529</t>
+  </si>
+  <si>
+    <t>MLR-50530</t>
+  </si>
+  <si>
+    <t>MLR-50531</t>
+  </si>
+  <si>
+    <t>MLR-50532</t>
+  </si>
+  <si>
+    <t>new case for Multi-layer rounding</t>
   </si>
 </sst>
 </file>
@@ -2492,13 +2531,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A5B6F5-D95C-4060-89B9-FDDC3DEF8E41}">
-  <dimension ref="A1:U576"/>
+  <dimension ref="A1:U590"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C440" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C558" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A459" sqref="A459:XFD459"/>
+      <selection pane="bottomRight" activeCell="G579" sqref="G579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,6 +2552,7 @@
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -2568,7 +2608,9 @@
       <c r="R1" s="24">
         <v>44533</v>
       </c>
-      <c r="S1" s="23"/>
+      <c r="S1" s="24">
+        <v>44543</v>
+      </c>
       <c r="T1" s="23"/>
       <c r="U1" s="25"/>
     </row>
@@ -21061,42 +21103,187 @@
       <c r="J570" s="3" t="s">
         <v>539</v>
       </c>
+      <c r="S570" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="571" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A571" s="13">
         <v>569</v>
       </c>
+      <c r="B571" s="2" t="s">
+        <v>552</v>
+      </c>
       <c r="C571" s="3"/>
+      <c r="S571" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="572" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A572" s="12">
         <v>570</v>
       </c>
+      <c r="B572" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="C572" s="3"/>
+      <c r="S572" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="573" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A573" s="13">
         <v>571</v>
       </c>
+      <c r="B573" s="2" t="s">
+        <v>554</v>
+      </c>
       <c r="C573" s="3"/>
+      <c r="S573" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="574" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A574" s="12">
         <v>572</v>
       </c>
+      <c r="B574" s="2" t="s">
+        <v>555</v>
+      </c>
       <c r="C574" s="3"/>
+      <c r="S574" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="575" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A575" s="13">
         <v>573</v>
       </c>
+      <c r="B575" s="2" t="s">
+        <v>556</v>
+      </c>
       <c r="C575" s="3"/>
+      <c r="S575" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="576" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A576" s="12">
         <v>574</v>
       </c>
+      <c r="B576" s="2" t="s">
+        <v>557</v>
+      </c>
       <c r="C576" s="3"/>
+      <c r="S576" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="577" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A577" s="13">
+        <v>575</v>
+      </c>
+      <c r="B577" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="S577" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="578" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A578" s="12">
+        <v>576</v>
+      </c>
+      <c r="B578" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="S578" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="579" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A579" s="13">
+        <v>577</v>
+      </c>
+      <c r="B579" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="S579" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="580" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A580" s="12">
+        <v>578</v>
+      </c>
+      <c r="B580" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="S580" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="581" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A581" s="13">
+        <v>579</v>
+      </c>
+      <c r="B581" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="S581" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="582" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A582" s="12">
+        <v>580</v>
+      </c>
+      <c r="B582" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="S582" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="583" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A583" s="13">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="584" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A584" s="12">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="585" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A585" s="13">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="586" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A586" s="12">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="587" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A587" s="13">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="588" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A588" s="12">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="589" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A589" s="13">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="590" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A590" s="12">
+        <v>588</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:U576" xr:uid="{976D048D-26A2-4D77-A964-2445B5CE5606}"/>

</xml_diff>